<commit_message>
Finished BOM file with a few questions inserted in the Excel file.
</commit_message>
<xml_diff>
--- a/hardware/MainBoard/MainBoard_BOM.xlsx
+++ b/hardware/MainBoard/MainBoard_BOM.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="346">
   <si>
     <t>Item #</t>
   </si>
@@ -109,6 +109,9 @@
     <t>FTDI</t>
   </si>
   <si>
+    <t>IC HS USB TO UART/FIFO 48LQFP</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
@@ -331,6 +334,9 @@
     <t>R56</t>
   </si>
   <si>
+    <t>49.9</t>
+  </si>
+  <si>
     <t>R33, R34, R35, R36</t>
   </si>
   <si>
@@ -373,6 +379,9 @@
     <t>93LC56BT-I/OT</t>
   </si>
   <si>
+    <t>100</t>
+  </si>
+  <si>
     <t>R66, R72, R73</t>
   </si>
   <si>
@@ -817,9 +826,6 @@
     <t>RJ45 connector</t>
   </si>
   <si>
-    <t>Out of stock at digi-key</t>
-  </si>
-  <si>
     <t>MEZZANINE 1MM BTB RECPT 84CKT</t>
   </si>
   <si>
@@ -839,13 +845,262 @@
   </si>
   <si>
     <t>LED 3X1MM 601NM ORN RA CHIP SMD</t>
+  </si>
+  <si>
+    <t>Fairchild Semiconductor</t>
+  </si>
+  <si>
+    <t>MMBT3904FSCT-ND</t>
+  </si>
+  <si>
+    <t>TRANSISTOR GP NPN AMP SOT-23</t>
+  </si>
+  <si>
+    <t>MCR01MRTF1002</t>
+  </si>
+  <si>
+    <t>Rohm</t>
+  </si>
+  <si>
+    <t>RHM10.0KCDCT-ND</t>
+  </si>
+  <si>
+    <t>RES 10.0K OHM 1/16W 1% 0402 SMD</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
+    <t>CRCW040224R9FKED</t>
+  </si>
+  <si>
+    <t>541-24.9LCT-ND</t>
+  </si>
+  <si>
+    <t>RES 24.9 OHM 1/16W 1% 0402 SMD</t>
+  </si>
+  <si>
+    <t>TRR01MZPF1003</t>
+  </si>
+  <si>
+    <t>RHM100KBHCT-ND</t>
+  </si>
+  <si>
+    <t>RES 100K OHM 1/16W 1% 0402 SMD</t>
+  </si>
+  <si>
+    <t>MCR01MZPF39R0</t>
+  </si>
+  <si>
+    <t>RHM39.0LCT-ND</t>
+  </si>
+  <si>
+    <t>RES 39.0 OHM 1/16W 1% 0402 SMD</t>
+  </si>
+  <si>
+    <t>TRR01MZPF1501</t>
+  </si>
+  <si>
+    <t>RHM1.50KBHCT-ND</t>
+  </si>
+  <si>
+    <t>RES 1.50K OHM 1/16W 1% 0402 SMD</t>
+  </si>
+  <si>
+    <t>TRR01MZPF1000</t>
+  </si>
+  <si>
+    <t>RES 100 OHM 1/16W 1% 0402 SMD</t>
+  </si>
+  <si>
+    <t>RHM100BHCT-ND</t>
+  </si>
+  <si>
+    <t>MCR01MRTF49R9</t>
+  </si>
+  <si>
+    <t>RHM49.9CDCT-ND</t>
+  </si>
+  <si>
+    <t>RES 49.9 OHM 1/16W 1% 0402 SMD</t>
+  </si>
+  <si>
+    <t>RES 22.0 OHM 1/16W 1% 0402 SMD</t>
+  </si>
+  <si>
+    <t>MCR01MRTF22R0</t>
+  </si>
+  <si>
+    <t>RHM22.0CDCT-ND</t>
+  </si>
+  <si>
+    <t>TRR01MZPJ000</t>
+  </si>
+  <si>
+    <t>RHM0.0BICT-ND</t>
+  </si>
+  <si>
+    <t>RES 0.0 OHM 1/16W 0402 SMD</t>
+  </si>
+  <si>
+    <t>MCR01MRTF2201</t>
+  </si>
+  <si>
+    <t>RHM2.20KCDCT-ND</t>
+  </si>
+  <si>
+    <t>RES 2.20K OHM 1/16W 1% 0402 SMD</t>
+  </si>
+  <si>
+    <t>TRR01MZPF1001</t>
+  </si>
+  <si>
+    <t>RHM1.00KBHCT-ND</t>
+  </si>
+  <si>
+    <t>RES 1.00K OHM 1/16W 1% 0402 SMD</t>
+  </si>
+  <si>
+    <t>CRCW04024R87FKED</t>
+  </si>
+  <si>
+    <t>541-4.87LLCT-ND</t>
+  </si>
+  <si>
+    <t>RES 4.87 OHM 1/16W 1% 0402 SMD</t>
+  </si>
+  <si>
+    <t>CRCW040212K0FKED</t>
+  </si>
+  <si>
+    <t>541-12.0KLCT-ND</t>
+  </si>
+  <si>
+    <t>RES 12.0K OHM 1/16W 1% 0402 SMD</t>
+  </si>
+  <si>
+    <t>CRCW040227R0FKED</t>
+  </si>
+  <si>
+    <t>541-27.0LCT-ND</t>
+  </si>
+  <si>
+    <t>RES 27.0 OHM 1/16W 1% 0402 SMD</t>
+  </si>
+  <si>
+    <t>CRCW040239K0FKED</t>
+  </si>
+  <si>
+    <t>541-39.0KLCT-ND</t>
+  </si>
+  <si>
+    <t>RES 39.0K OHM 1/16W 1% 0402 SMD</t>
+  </si>
+  <si>
+    <t>CRCW04022K00FKED</t>
+  </si>
+  <si>
+    <t>541-2.00KLCT-ND</t>
+  </si>
+  <si>
+    <t>RES 2.00K OHM 1/16W 1% 0402 SMD</t>
+  </si>
+  <si>
+    <t>CRCW0402100RFKED</t>
+  </si>
+  <si>
+    <t>541-100LCT-ND</t>
+  </si>
+  <si>
+    <t>CRCW0402330RFKED</t>
+  </si>
+  <si>
+    <t>541-330LCT-ND</t>
+  </si>
+  <si>
+    <t>RES 330 OHM 1/16W 1% 0402 SMD</t>
+  </si>
+  <si>
+    <t>CRCW04024K70FKED</t>
+  </si>
+  <si>
+    <t>541-4.70KLCT-ND</t>
+  </si>
+  <si>
+    <t>RES 4.70K OHM 1/16W 1% 0402 SMD</t>
+  </si>
+  <si>
+    <t>TL3340AF160QG</t>
+  </si>
+  <si>
+    <t>EG4627CT-ND</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO 0.05A 12V</t>
+  </si>
+  <si>
+    <t>E-Switch</t>
+  </si>
+  <si>
+    <t>TEST POINT PC COMPACT .063"D YLW</t>
+  </si>
+  <si>
+    <t>TEST POINT PC COMPACT T/H GREEN</t>
+  </si>
+  <si>
+    <t>IC FPGA 512K FLASH 256FPBGA</t>
+  </si>
+  <si>
+    <t>IC ANLG FRNT END 48-TQFN</t>
+  </si>
+  <si>
+    <t>IC TXRX ETHERNET PHYTER 48-LQFP</t>
+  </si>
+  <si>
+    <t>IC EEPROM 2KBIT 3MHZ SOT23-6</t>
+  </si>
+  <si>
+    <t>IC ECONRST 3.3V W/PB 10% SOT23-3</t>
+  </si>
+  <si>
+    <t>CRYSTAL 16.000 MHZ 8PF SMD</t>
+  </si>
+  <si>
+    <t>CRYSTAL 32.768 KHZ 7PF SMD</t>
+  </si>
+  <si>
+    <t>OSC MEMS 50.000 MHZ 3.3V SMD</t>
+  </si>
+  <si>
+    <t>CRYSTAL 12.000 MHZ 9PF SMD</t>
+  </si>
+  <si>
+    <t>STANDOFF HEX M/F .375"L 4-40 BR</t>
+  </si>
+  <si>
+    <t>7200K-ND</t>
+  </si>
+  <si>
+    <t>INDUCTOR CHIP 33NH 5% SMD</t>
+  </si>
+  <si>
+    <t>PM0603-33NJ-RC</t>
+  </si>
+  <si>
+    <t>JW Miller</t>
+  </si>
+  <si>
+    <t>M8487CT-ND</t>
+  </si>
+  <si>
+    <t>Out of stock at digi-key, do we have it in house? Should we go Mouser?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -895,14 +1150,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1004,12 +1251,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1062,17 +1308,16 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="4" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
-    <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
@@ -1381,7 +1626,7 @@
   <dimension ref="A1:M63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1460,28 +1705,28 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>92</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="I4" s="17" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="J4" s="1">
         <v>1</v>
@@ -1499,28 +1744,28 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="J5" s="1">
         <v>3</v>
@@ -1538,28 +1783,28 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>57</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>215</v>
+        <v>220</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>218</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="J6" s="1">
         <v>17</v>
@@ -1571,8 +1816,8 @@
         <f t="shared" si="0"/>
         <v>5.0999999999999996</v>
       </c>
-      <c r="M6" s="22" t="s">
-        <v>235</v>
+      <c r="M6" s="21" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1580,28 +1825,28 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>43</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="J7" s="1">
         <v>73</v>
@@ -1619,22 +1864,22 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="21" t="s">
-        <v>75</v>
-      </c>
       <c r="D8" s="19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J8" s="1">
         <v>7</v>
@@ -1643,8 +1888,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M8" s="22" t="s">
-        <v>224</v>
+      <c r="M8" s="21" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1652,28 +1897,28 @@
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>41</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="J9" s="1">
         <v>3</v>
@@ -1691,28 +1936,28 @@
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>73</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="J10" s="1">
         <v>4</v>
@@ -1730,28 +1975,28 @@
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>67</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="J11" s="1">
         <v>2</v>
@@ -1769,25 +2014,25 @@
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C12" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="I12" s="17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J12" s="1">
         <v>1</v>
@@ -1796,8 +2041,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M12" s="22" t="s">
-        <v>234</v>
+      <c r="M12" s="21" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1805,28 +2050,28 @@
         <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>45</v>
-      </c>
       <c r="D13" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="J13" s="1">
         <v>7</v>
@@ -1844,20 +2089,20 @@
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="14" t="s">
         <v>24</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>23</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
       <c r="I14" s="18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J14" s="14">
         <v>18</v>
@@ -1872,28 +2117,28 @@
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>80</v>
-      </c>
       <c r="D15" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="J15" s="1">
         <v>8</v>
@@ -1911,28 +2156,28 @@
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="J16" s="1">
         <v>2</v>
@@ -1950,28 +2195,28 @@
         <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>71</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="J17" s="1">
         <v>2</v>
@@ -1989,28 +2234,28 @@
         <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>63</v>
-      </c>
       <c r="D18" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="J18" s="1">
         <v>4</v>
@@ -2028,28 +2273,28 @@
         <v>16</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="J19" s="1">
         <v>1</v>
@@ -2067,28 +2312,28 @@
         <v>17</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="J20" s="1">
         <v>1</v>
@@ -2106,28 +2351,28 @@
         <v>18</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="J21" s="1">
         <v>1</v>
@@ -2139,8 +2384,8 @@
         <f t="shared" si="0"/>
         <v>3.45</v>
       </c>
-      <c r="M21" s="22" t="s">
-        <v>253</v>
+      <c r="M21" s="21" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -2148,28 +2393,28 @@
         <v>19</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="J22" s="1">
         <v>1</v>
@@ -2187,28 +2432,28 @@
         <v>20</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="F23" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="J23" s="1">
         <v>1</v>
@@ -2226,28 +2471,28 @@
         <v>21</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="J24" s="1">
         <v>1</v>
@@ -2265,16 +2510,28 @@
         <v>22</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>85</v>
+      <c r="E25" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>344</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>87</v>
+        <v>341</v>
       </c>
       <c r="J25" s="1">
         <v>2</v>
@@ -2289,28 +2546,28 @@
         <v>23</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="D26" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="I26" s="17" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="J26" s="1">
         <v>1</v>
@@ -2328,28 +2585,28 @@
         <v>24</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D27" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="I27" s="17" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J27" s="1">
         <v>1</v>
@@ -2367,25 +2624,38 @@
         <v>25</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="G28" s="14"/>
+        <v>193</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>264</v>
+      </c>
       <c r="I28" s="17" t="s">
-        <v>192</v>
+        <v>265</v>
       </c>
       <c r="J28" s="1">
         <v>1</v>
       </c>
-      <c r="K28" s="2"/>
+      <c r="K28">
+        <v>0.37</v>
+      </c>
       <c r="L28" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="29" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2393,28 +2663,38 @@
         <v>26</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="15" t="s">
-        <v>69</v>
-      </c>
       <c r="D29" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>268</v>
+      </c>
       <c r="I29" s="17" t="s">
-        <v>37</v>
+        <v>269</v>
       </c>
       <c r="J29" s="1">
         <v>6</v>
       </c>
-      <c r="K29"/>
+      <c r="K29">
+        <v>2.3E-2</v>
+      </c>
       <c r="L29" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.13800000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -2422,23 +2702,38 @@
         <v>27</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C30" s="15">
         <v>24.9</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>37</v>
+        <v>273</v>
       </c>
       <c r="J30" s="1">
         <v>8</v>
       </c>
+      <c r="K30">
+        <v>8.3000000000000004E-2</v>
+      </c>
       <c r="L30" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.66400000000000003</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -2446,23 +2741,38 @@
         <v>28</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>275</v>
       </c>
       <c r="I31" s="17" t="s">
-        <v>37</v>
+        <v>276</v>
       </c>
       <c r="J31" s="1">
         <v>6</v>
       </c>
+      <c r="K31">
+        <v>0.123</v>
+      </c>
       <c r="L31" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.73799999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -2470,23 +2780,38 @@
         <v>29</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C32" s="15">
         <v>39</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>278</v>
       </c>
       <c r="I32" s="17" t="s">
-        <v>37</v>
+        <v>279</v>
       </c>
       <c r="J32" s="1">
         <v>7</v>
       </c>
+      <c r="K32">
+        <v>2.5999999999999999E-2</v>
+      </c>
       <c r="L32" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.182</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2494,23 +2819,38 @@
         <v>30</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="15" t="s">
-        <v>47</v>
-      </c>
       <c r="D33" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>281</v>
       </c>
       <c r="I33" s="17" t="s">
-        <v>37</v>
+        <v>282</v>
       </c>
       <c r="J33" s="1">
         <v>1</v>
       </c>
+      <c r="K33">
+        <v>0.123</v>
+      </c>
       <c r="L33" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.123</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2518,23 +2858,38 @@
         <v>31</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C34" s="15">
-        <v>110</v>
+        <v>111</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>107</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>285</v>
       </c>
       <c r="I34" s="17" t="s">
-        <v>37</v>
+        <v>284</v>
       </c>
       <c r="J34" s="1">
         <v>2</v>
       </c>
+      <c r="K34">
+        <v>0.20100000000000001</v>
+      </c>
       <c r="L34" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.40200000000000002</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2542,23 +2897,38 @@
         <v>32</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C35" s="15">
-        <v>49.9</v>
+        <v>93</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>287</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>37</v>
+        <v>288</v>
       </c>
       <c r="J35" s="1">
         <v>4</v>
       </c>
+      <c r="K35">
+        <v>2.3E-2</v>
+      </c>
       <c r="L35" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.1999999999999998E-2</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2566,23 +2936,38 @@
         <v>33</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C36" s="15">
         <v>22</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>291</v>
       </c>
       <c r="I36" s="17" t="s">
-        <v>37</v>
+        <v>289</v>
       </c>
       <c r="J36" s="1">
         <v>7</v>
       </c>
+      <c r="K36">
+        <v>2.3E-2</v>
+      </c>
       <c r="L36" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.161</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2590,23 +2975,38 @@
         <v>34</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C37" s="15">
         <v>0</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>293</v>
       </c>
       <c r="I37" s="17" t="s">
-        <v>37</v>
+        <v>294</v>
       </c>
       <c r="J37" s="1">
         <v>12</v>
       </c>
+      <c r="K37">
+        <v>0.18099999999999999</v>
+      </c>
       <c r="L37" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.1719999999999997</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2614,23 +3014,38 @@
         <v>35</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="15" t="s">
-        <v>51</v>
-      </c>
       <c r="D38" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>296</v>
       </c>
       <c r="I38" s="17" t="s">
-        <v>37</v>
+        <v>297</v>
       </c>
       <c r="J38" s="1">
         <v>7</v>
       </c>
+      <c r="K38">
+        <v>2.3E-2</v>
+      </c>
       <c r="L38" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.161</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2638,23 +3053,38 @@
         <v>36</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C39" s="15" t="s">
-        <v>49</v>
-      </c>
       <c r="D39" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>299</v>
       </c>
       <c r="I39" s="17" t="s">
-        <v>37</v>
+        <v>300</v>
       </c>
       <c r="J39" s="1">
         <v>4</v>
       </c>
+      <c r="K39">
+        <v>0.123</v>
+      </c>
       <c r="L39" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.49199999999999999</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2662,23 +3092,38 @@
         <v>37</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C40" s="15" t="s">
-        <v>65</v>
-      </c>
       <c r="D40" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>302</v>
       </c>
       <c r="I40" s="17" t="s">
-        <v>37</v>
+        <v>303</v>
       </c>
       <c r="J40" s="1">
         <v>1</v>
       </c>
+      <c r="K40">
+        <v>8.3000000000000004E-2</v>
+      </c>
       <c r="L40" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3000000000000004E-2</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2686,23 +3131,38 @@
         <v>38</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="15" t="s">
-        <v>77</v>
-      </c>
       <c r="D41" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>305</v>
       </c>
       <c r="I41" s="17" t="s">
-        <v>37</v>
+        <v>306</v>
       </c>
       <c r="J41" s="1">
         <v>1</v>
       </c>
+      <c r="K41">
+        <v>8.3000000000000004E-2</v>
+      </c>
       <c r="L41" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3000000000000004E-2</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -2710,23 +3170,38 @@
         <v>39</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C42" s="15">
         <v>27</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>308</v>
       </c>
       <c r="I42" s="17" t="s">
-        <v>37</v>
+        <v>309</v>
       </c>
       <c r="J42" s="1">
         <v>1</v>
       </c>
+      <c r="K42">
+        <v>8.3000000000000004E-2</v>
+      </c>
       <c r="L42" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3000000000000004E-2</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -2734,23 +3209,38 @@
         <v>40</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C43" s="15" t="s">
-        <v>89</v>
-      </c>
       <c r="D43" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="I43" s="17" t="s">
-        <v>37</v>
+        <v>312</v>
       </c>
       <c r="J43" s="1">
         <v>1</v>
       </c>
+      <c r="K43">
+        <v>8.3000000000000004E-2</v>
+      </c>
       <c r="L43" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3000000000000004E-2</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -2758,23 +3248,38 @@
         <v>41</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="15" t="s">
-        <v>59</v>
-      </c>
       <c r="D44" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>314</v>
       </c>
       <c r="I44" s="17" t="s">
-        <v>37</v>
+        <v>315</v>
       </c>
       <c r="J44" s="1">
         <v>1</v>
       </c>
+      <c r="K44">
+        <v>8.3000000000000004E-2</v>
+      </c>
       <c r="L44" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3000000000000004E-2</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -2782,23 +3287,38 @@
         <v>42</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C45" s="15">
         <v>100</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>317</v>
       </c>
       <c r="I45" s="17" t="s">
-        <v>37</v>
+        <v>284</v>
       </c>
       <c r="J45" s="1">
         <v>3</v>
       </c>
+      <c r="K45">
+        <v>8.3000000000000004E-2</v>
+      </c>
       <c r="L45" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.249</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -2806,23 +3326,38 @@
         <v>43</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C46" s="15">
         <v>330</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>319</v>
       </c>
       <c r="I46" s="17" t="s">
-        <v>37</v>
+        <v>320</v>
       </c>
       <c r="J46" s="1">
         <v>1</v>
       </c>
+      <c r="K46">
+        <v>8.3000000000000004E-2</v>
+      </c>
       <c r="L46" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3000000000000004E-2</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -2830,23 +3365,38 @@
         <v>44</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C47" s="15" t="s">
-        <v>61</v>
-      </c>
       <c r="D47" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>322</v>
       </c>
       <c r="I47" s="17" t="s">
-        <v>37</v>
+        <v>323</v>
       </c>
       <c r="J47" s="1">
         <v>2</v>
       </c>
+      <c r="K47">
+        <v>8.3000000000000004E-2</v>
+      </c>
       <c r="L47" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.16600000000000001</v>
       </c>
     </row>
     <row r="48" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2854,20 +3404,20 @@
         <v>45</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D48" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C48" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D48" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E48" s="14"/>
+      <c r="E48" s="1"/>
       <c r="F48" s="14"/>
       <c r="G48" s="14"/>
       <c r="H48" s="14"/>
       <c r="I48" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J48" s="14">
         <v>1</v>
@@ -2882,28 +3432,38 @@
         <v>46</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
+        <v>201</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>325</v>
+      </c>
       <c r="I49" s="17" t="s">
-        <v>200</v>
+        <v>326</v>
       </c>
       <c r="J49" s="1">
         <v>2</v>
       </c>
-      <c r="K49"/>
+      <c r="K49">
+        <v>0.29099999999999998</v>
+      </c>
       <c r="L49" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.58199999999999996</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -2911,16 +3471,16 @@
         <v>47</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="F50" s="1">
         <v>5009</v>
@@ -2929,17 +3489,20 @@
         <v>11</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="I50" s="17" t="s">
-        <v>203</v>
+        <v>328</v>
       </c>
       <c r="J50" s="1">
         <v>2</v>
       </c>
+      <c r="K50">
+        <v>0.35</v>
+      </c>
       <c r="L50" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -2947,16 +3510,16 @@
         <v>48</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="F51" s="1">
         <v>5121</v>
@@ -2965,17 +3528,20 @@
         <v>11</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="I51" s="17" t="s">
-        <v>203</v>
+        <v>329</v>
       </c>
       <c r="J51" s="1">
         <v>2</v>
       </c>
+      <c r="K51">
+        <v>0.35</v>
+      </c>
       <c r="L51" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -2986,32 +3552,35 @@
         <v>12</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E52" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="G52" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="I52" s="17" t="s">
-        <v>118</v>
+        <v>330</v>
       </c>
       <c r="J52" s="1">
         <v>1</v>
       </c>
+      <c r="K52">
+        <v>53.91</v>
+      </c>
       <c r="L52" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>53.91</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -3019,35 +3588,38 @@
         <v>50</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="I53" s="17" t="s">
-        <v>187</v>
+        <v>331</v>
       </c>
       <c r="J53" s="1">
         <v>2</v>
       </c>
+      <c r="K53">
+        <v>20.09</v>
+      </c>
       <c r="L53" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40.18</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -3055,35 +3627,38 @@
         <v>51</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H54" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="I54" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="I54" s="17" t="s">
-        <v>211</v>
-      </c>
       <c r="J54" s="1">
         <v>1</v>
       </c>
+      <c r="K54">
+        <v>0.95</v>
+      </c>
       <c r="L54" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -3091,13 +3666,13 @@
         <v>52</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>16</v>
@@ -3112,14 +3687,17 @@
         <v>15</v>
       </c>
       <c r="I55" s="17" t="s">
-        <v>183</v>
+        <v>17</v>
       </c>
       <c r="J55" s="1">
         <v>1</v>
       </c>
+      <c r="K55">
+        <v>4.25</v>
+      </c>
       <c r="L55" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -3127,35 +3705,38 @@
         <v>53</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="I56" s="17" t="s">
-        <v>156</v>
+        <v>332</v>
       </c>
       <c r="J56" s="1">
         <v>1</v>
       </c>
+      <c r="K56">
+        <v>6.66</v>
+      </c>
       <c r="L56" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.66</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -3163,36 +3744,38 @@
         <v>54</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F57" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H57" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G57" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="I57" s="17" t="s">
-        <v>101</v>
+        <v>333</v>
       </c>
       <c r="J57" s="1">
         <v>1</v>
       </c>
-      <c r="K57" s="2"/>
+      <c r="K57">
+        <v>0.34</v>
+      </c>
       <c r="L57" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="58" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3200,36 +3783,38 @@
         <v>55</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="I58" s="17" t="s">
-        <v>162</v>
+        <v>334</v>
       </c>
       <c r="J58" s="1">
         <v>1</v>
       </c>
-      <c r="K58"/>
+      <c r="K58">
+        <v>0.81</v>
+      </c>
       <c r="L58" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
@@ -3237,36 +3822,38 @@
         <v>56</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="I59" s="17" t="s">
-        <v>178</v>
+        <v>335</v>
       </c>
       <c r="J59" s="1">
         <v>1</v>
       </c>
-      <c r="K59" s="2"/>
+      <c r="K59">
+        <v>4.3099999999999996</v>
+      </c>
       <c r="L59" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.3099999999999996</v>
       </c>
     </row>
     <row r="60" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3274,35 +3861,38 @@
         <v>57</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="I60" s="17" t="s">
-        <v>166</v>
+        <v>336</v>
       </c>
       <c r="J60" s="1">
         <v>1</v>
       </c>
+      <c r="K60">
+        <v>1.58</v>
+      </c>
       <c r="L60" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="61" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3310,35 +3900,38 @@
         <v>58</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="I61" s="17" t="s">
-        <v>123</v>
+        <v>337</v>
       </c>
       <c r="J61" s="1">
         <v>1</v>
       </c>
+      <c r="K61">
+        <v>2.59</v>
+      </c>
       <c r="L61" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.59</v>
       </c>
     </row>
     <row r="62" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3346,36 +3939,38 @@
         <v>59</v>
       </c>
       <c r="B62" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C62" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="F62" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="I62" s="17" t="s">
-        <v>173</v>
+        <v>338</v>
       </c>
       <c r="J62" s="1">
         <v>1</v>
       </c>
-      <c r="K62"/>
+      <c r="K62">
+        <v>2.06</v>
+      </c>
       <c r="L62" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.06</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
@@ -3383,23 +3978,38 @@
         <v>60</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F63" s="1">
+        <v>7200</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>340</v>
       </c>
       <c r="I63" s="17" t="s">
-        <v>194</v>
+        <v>339</v>
       </c>
       <c r="J63" s="1">
         <v>4</v>
       </c>
+      <c r="K63">
+        <v>0.68</v>
+      </c>
       <c r="L63" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.72</v>
       </c>
     </row>
   </sheetData>
@@ -3447,905 +4057,905 @@
         <v>8</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>92</v>
-      </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="J2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D3">
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="H3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="J3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>57</v>
-      </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4">
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>43</v>
-      </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5">
         <v>73</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>75</v>
-      </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6">
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>41</v>
-      </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>73</v>
-      </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D8">
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>67</v>
-      </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>53</v>
-      </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>45</v>
-      </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D11">
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
         <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
       </c>
       <c r="D12">
         <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>80</v>
-      </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D13">
         <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D14">
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>71</v>
-      </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D15">
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>63</v>
-      </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D16">
         <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C17" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C18" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F18" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="H18" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="J18" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C19" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F19" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="H19" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="J19" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C20" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="F20" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H20" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="J20" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>132</v>
+      </c>
+      <c r="F21" t="s">
+        <v>138</v>
+      </c>
+      <c r="H21" t="s">
         <v>134</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="C21" t="s">
-        <v>133</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>129</v>
-      </c>
-      <c r="F21" t="s">
-        <v>135</v>
-      </c>
-      <c r="H21" t="s">
-        <v>131</v>
-      </c>
       <c r="J21" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C22" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="F22" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H22" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="J22" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" t="s">
         <v>86</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" t="s">
-        <v>85</v>
       </c>
       <c r="D23">
         <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" t="s">
         <v>33</v>
       </c>
-      <c r="C24" t="s">
-        <v>32</v>
-      </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
         <v>28</v>
       </c>
-      <c r="C25" t="s">
-        <v>27</v>
-      </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C26" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="10" t="s">
-        <v>69</v>
-      </c>
       <c r="C27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D27">
         <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B28" s="10">
         <v>24.9</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D28">
         <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C29" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D29">
         <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B30" s="10">
         <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D30">
         <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>47</v>
-      </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B32" s="10">
         <v>110</v>
       </c>
       <c r="C32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D32">
         <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B33" s="10">
         <v>49.9</v>
       </c>
       <c r="C33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D33">
         <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B34" s="10">
         <v>22</v>
       </c>
       <c r="C34" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D34">
         <v>7</v>
       </c>
       <c r="E34" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B35" s="10">
         <v>0</v>
       </c>
       <c r="C35" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D35">
         <v>12</v>
       </c>
       <c r="E35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B36" s="10" t="s">
-        <v>51</v>
-      </c>
       <c r="C36" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D36">
         <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="10" t="s">
-        <v>49</v>
-      </c>
       <c r="C37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D37">
         <v>4</v>
       </c>
       <c r="E37" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="10" t="s">
-        <v>65</v>
-      </c>
       <c r="C38" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B39" s="10" t="s">
-        <v>77</v>
-      </c>
       <c r="C39" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B40" s="10">
         <v>27</v>
       </c>
       <c r="C40" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B41" s="10" t="s">
-        <v>89</v>
-      </c>
       <c r="C41" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B42" s="10" t="s">
-        <v>59</v>
-      </c>
       <c r="C42" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B43" s="10">
         <v>100</v>
       </c>
       <c r="C43" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D43">
         <v>3</v>
       </c>
       <c r="E43" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B44" s="10">
         <v>330</v>
       </c>
       <c r="C44" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B45" s="10" t="s">
-        <v>61</v>
-      </c>
       <c r="C45" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D45">
         <v>2</v>
       </c>
       <c r="E45" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B46" s="10">
         <v>0</v>
       </c>
       <c r="C46" t="s">
+        <v>39</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
         <v>38</v>
       </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-      <c r="E46" t="s">
-        <v>37</v>
-      </c>
       <c r="G46" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C47" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D47">
         <v>2</v>
       </c>
       <c r="E47" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C48" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D48">
         <v>2</v>
       </c>
       <c r="E48" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="F48" t="s">
+        <v>211</v>
+      </c>
+      <c r="H48" t="s">
         <v>208</v>
-      </c>
-      <c r="H48" t="s">
-        <v>205</v>
       </c>
       <c r="J48">
         <v>5009</v>
@@ -4353,25 +4963,25 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C49" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D49">
         <v>2</v>
       </c>
       <c r="E49" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="F49" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="H49" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="J49">
         <v>5121</v>
@@ -4382,94 +4992,94 @@
         <v>12</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C50" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D50">
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F50" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="H50" t="s">
+        <v>123</v>
+      </c>
+      <c r="J50" t="s">
         <v>120</v>
-      </c>
-      <c r="J50" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C51" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D51">
         <v>2</v>
       </c>
       <c r="E51" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F51" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="H51" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="J51" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C52" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D52">
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="F52" t="s">
+        <v>215</v>
+      </c>
+      <c r="H52" t="s">
+        <v>216</v>
+      </c>
+      <c r="J52" t="s">
         <v>212</v>
-      </c>
-      <c r="H52" t="s">
-        <v>213</v>
-      </c>
-      <c r="J52" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C53" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D53">
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="F53" t="s">
         <v>15</v>
@@ -4478,7 +5088,7 @@
         <v>16</v>
       </c>
       <c r="I53" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="J53" t="s">
         <v>15</v>
@@ -4486,201 +5096,201 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C54" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D54">
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F54" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="H54" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="J54" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C55" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D55">
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F55" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H55" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J55" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C56" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D56">
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="F56" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="H56" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="J56" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C57" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="F57" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="H57" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="J57" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C58" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="F58" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H58" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="J58" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C59" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D59">
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="F59" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="H59" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="J59" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>175</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C60" t="s">
+        <v>174</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60" t="s">
+        <v>176</v>
+      </c>
+      <c r="F60" t="s">
+        <v>177</v>
+      </c>
+      <c r="H60" t="s">
         <v>172</v>
       </c>
-      <c r="B60" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="C60" t="s">
-        <v>171</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="E60" t="s">
-        <v>173</v>
-      </c>
-      <c r="F60" t="s">
-        <v>174</v>
-      </c>
-      <c r="H60" t="s">
-        <v>169</v>
-      </c>
       <c r="J60" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C61" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D61">
         <v>4</v>
       </c>
       <c r="E61" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reorganized names on board for better visibility on assembly diagrams.
</commit_message>
<xml_diff>
--- a/hardware/MainBoard/MainBoard_BOM.xlsx
+++ b/hardware/MainBoard/MainBoard_BOM.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="347">
   <si>
     <t>Item #</t>
   </si>
@@ -1094,6 +1094,9 @@
   </si>
   <si>
     <t>Out of stock at digi-key, do we have it in house? Should we go Mouser?</t>
+  </si>
+  <si>
+    <t>SW3</t>
   </si>
 </sst>
 </file>
@@ -1274,12 +1277,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1313,6 +1310,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1626,7 +1629,7 @@
   <dimension ref="A1:M63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1647,20 +1650,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -1707,7 +1710,7 @@
       <c r="B4" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="13" t="s">
         <v>94</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1725,7 +1728,7 @@
       <c r="H4" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="15" t="s">
         <v>226</v>
       </c>
       <c r="J4" s="1">
@@ -1746,7 +1749,7 @@
       <c r="B5" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="13" t="s">
         <v>113</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1764,7 +1767,7 @@
       <c r="H5" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="15" t="s">
         <v>225</v>
       </c>
       <c r="J5" s="1">
@@ -1785,7 +1788,7 @@
       <c r="B6" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="13" t="s">
         <v>58</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1794,7 +1797,7 @@
       <c r="E6" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="20" t="s">
         <v>218</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -1803,7 +1806,7 @@
       <c r="H6" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="15" t="s">
         <v>224</v>
       </c>
       <c r="J6" s="1">
@@ -1816,7 +1819,7 @@
         <f t="shared" si="0"/>
         <v>5.0999999999999996</v>
       </c>
-      <c r="M6" s="21" t="s">
+      <c r="M6" s="19" t="s">
         <v>238</v>
       </c>
     </row>
@@ -1827,7 +1830,7 @@
       <c r="B7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="13" t="s">
         <v>44</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1845,7 +1848,7 @@
       <c r="H7" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="15" t="s">
         <v>223</v>
       </c>
       <c r="J7" s="1">
@@ -1866,10 +1869,10 @@
       <c r="B8" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="17" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -1878,7 +1881,7 @@
       <c r="G8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="15" t="s">
         <v>26</v>
       </c>
       <c r="J8" s="1">
@@ -1888,7 +1891,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M8" s="21" t="s">
+      <c r="M8" s="19" t="s">
         <v>227</v>
       </c>
     </row>
@@ -1899,7 +1902,7 @@
       <c r="B9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="13" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1917,7 +1920,7 @@
       <c r="H9" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="15" t="s">
         <v>230</v>
       </c>
       <c r="J9" s="1">
@@ -1938,7 +1941,7 @@
       <c r="B10" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="13" t="s">
         <v>74</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1956,7 +1959,7 @@
       <c r="H10" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="15" t="s">
         <v>233</v>
       </c>
       <c r="J10" s="1">
@@ -1977,7 +1980,7 @@
       <c r="B11" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="13" t="s">
         <v>68</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1995,7 +1998,7 @@
       <c r="H11" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="15" t="s">
         <v>236</v>
       </c>
       <c r="J11" s="1">
@@ -2016,13 +2019,13 @@
       <c r="B12" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="17" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="4" t="s">
@@ -2031,7 +2034,7 @@
       <c r="H12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="I12" s="15" t="s">
         <v>26</v>
       </c>
       <c r="J12" s="1">
@@ -2041,7 +2044,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M12" s="21" t="s">
+      <c r="M12" s="19" t="s">
         <v>237</v>
       </c>
     </row>
@@ -2052,7 +2055,7 @@
       <c r="B13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="13" t="s">
         <v>46</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -2070,7 +2073,7 @@
       <c r="H13" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="I13" s="17" t="s">
+      <c r="I13" s="15" t="s">
         <v>241</v>
       </c>
       <c r="J13" s="1">
@@ -2085,26 +2088,26 @@
       </c>
     </row>
     <row r="14" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
+      <c r="A14" s="11">
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="18" t="s">
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="12">
         <v>18</v>
       </c>
       <c r="L14" s="6">
@@ -2119,7 +2122,7 @@
       <c r="B15" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="13" t="s">
         <v>81</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -2137,7 +2140,7 @@
       <c r="H15" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="I15" s="17" t="s">
+      <c r="I15" s="15" t="s">
         <v>244</v>
       </c>
       <c r="J15" s="1">
@@ -2158,7 +2161,7 @@
       <c r="B16" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="13" t="s">
         <v>118</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -2176,7 +2179,7 @@
       <c r="H16" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="I16" s="17" t="s">
+      <c r="I16" s="15" t="s">
         <v>247</v>
       </c>
       <c r="J16" s="1">
@@ -2197,7 +2200,7 @@
       <c r="B17" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="13" t="s">
         <v>72</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -2215,7 +2218,7 @@
       <c r="H17" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="I17" s="17" t="s">
+      <c r="I17" s="15" t="s">
         <v>230</v>
       </c>
       <c r="J17" s="1">
@@ -2236,7 +2239,7 @@
       <c r="B18" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="13" t="s">
         <v>64</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -2254,7 +2257,7 @@
       <c r="H18" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="I18" s="17" t="s">
+      <c r="I18" s="15" t="s">
         <v>249</v>
       </c>
       <c r="J18" s="1">
@@ -2268,43 +2271,43 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
-        <v>16</v>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>21</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="C19" s="15" t="s">
-        <v>198</v>
+      <c r="C19" s="13" t="s">
+        <v>152</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>251</v>
+        <v>152</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>252</v>
+        <v>156</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="G19" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="I19" s="17" t="s">
-        <v>200</v>
+        <v>155</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>154</v>
       </c>
       <c r="J19" s="1">
         <v>1</v>
       </c>
       <c r="K19">
-        <v>0.97</v>
+        <v>1.6</v>
       </c>
       <c r="L19" s="6">
-        <f t="shared" si="0"/>
-        <v>0.97</v>
+        <f>J19*K19</f>
+        <v>1.6</v>
       </c>
     </row>
     <row r="20" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2314,7 +2317,7 @@
       <c r="B20" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="13" t="s">
         <v>146</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -2332,7 +2335,7 @@
       <c r="H20" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I20" s="17" t="s">
+      <c r="I20" s="15" t="s">
         <v>255</v>
       </c>
       <c r="J20" s="1">
@@ -2353,7 +2356,7 @@
       <c r="B21" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="13" t="s">
         <v>140</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -2371,7 +2374,7 @@
       <c r="H21" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="I21" s="17" t="s">
+      <c r="I21" s="15" t="s">
         <v>257</v>
       </c>
       <c r="J21" s="1">
@@ -2384,7 +2387,7 @@
         <f t="shared" si="0"/>
         <v>3.45</v>
       </c>
-      <c r="M21" s="21" t="s">
+      <c r="M21" s="19" t="s">
         <v>345</v>
       </c>
     </row>
@@ -2395,7 +2398,7 @@
       <c r="B22" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="13" t="s">
         <v>130</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -2413,7 +2416,7 @@
       <c r="H22" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="I22" s="17" t="s">
+      <c r="I22" s="15" t="s">
         <v>256</v>
       </c>
       <c r="J22" s="1">
@@ -2434,7 +2437,7 @@
       <c r="B23" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="13" t="s">
         <v>136</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -2452,7 +2455,7 @@
       <c r="H23" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="I23" s="17" t="s">
+      <c r="I23" s="15" t="s">
         <v>258</v>
       </c>
       <c r="J23" s="1">
@@ -2468,283 +2471,283 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>152</v>
+        <v>87</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>85</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>152</v>
+        <v>86</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>156</v>
+        <v>343</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="G24" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="I24" s="17" t="s">
-        <v>154</v>
+        <v>344</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>341</v>
       </c>
       <c r="J24" s="1">
-        <v>1</v>
-      </c>
-      <c r="K24">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="L24" s="6">
         <f t="shared" si="0"/>
-        <v>1.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>85</v>
+        <v>34</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>86</v>
+        <v>33</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>343</v>
+        <v>31</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>342</v>
+        <v>35</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="I25" s="17" t="s">
-        <v>341</v>
+        <v>259</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>260</v>
       </c>
       <c r="J25" s="1">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>0.6</v>
       </c>
       <c r="L25" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="I26" s="17" t="s">
-        <v>260</v>
+        <v>261</v>
+      </c>
+      <c r="I26" s="15" t="s">
+        <v>262</v>
       </c>
       <c r="J26" s="1">
         <v>1</v>
       </c>
       <c r="K26">
-        <v>0.6</v>
+        <v>0.33</v>
       </c>
       <c r="L26" s="6">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>28</v>
+        <v>194</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>193</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>28</v>
+        <v>193</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>31</v>
+        <v>263</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>32</v>
+        <v>193</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="I27" s="17" t="s">
-        <v>262</v>
+        <v>264</v>
+      </c>
+      <c r="I27" s="15" t="s">
+        <v>265</v>
       </c>
       <c r="J27" s="1">
         <v>1</v>
       </c>
       <c r="K27">
-        <v>0.33</v>
+        <v>0.37</v>
       </c>
       <c r="L27" s="6">
         <f t="shared" si="0"/>
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>25</v>
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>26</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>193</v>
+        <v>71</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>193</v>
+        <v>36</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>193</v>
+        <v>266</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="I28" s="17" t="s">
-        <v>265</v>
+        <v>268</v>
+      </c>
+      <c r="I28" s="15" t="s">
+        <v>269</v>
       </c>
       <c r="J28" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K28">
-        <v>0.37</v>
+        <v>2.3E-2</v>
       </c>
       <c r="L28" s="6">
         <f t="shared" si="0"/>
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
-        <v>26</v>
+        <v>0.13800000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>70</v>
+        <v>83</v>
+      </c>
+      <c r="C29" s="13">
+        <v>24.9</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="I29" s="17" t="s">
-        <v>269</v>
+        <v>272</v>
+      </c>
+      <c r="I29" s="15" t="s">
+        <v>273</v>
       </c>
       <c r="J29" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K29">
-        <v>2.3E-2</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="L29" s="6">
         <f t="shared" si="0"/>
-        <v>0.13800000000000001</v>
+        <v>0.66400000000000003</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C30" s="15">
-        <v>24.9</v>
+        <v>110</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>109</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="I30" s="17" t="s">
-        <v>273</v>
+        <v>275</v>
+      </c>
+      <c r="I30" s="15" t="s">
+        <v>276</v>
       </c>
       <c r="J30" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K30">
-        <v>8.3000000000000004E-2</v>
+        <v>0.123</v>
       </c>
       <c r="L30" s="6">
         <f t="shared" si="0"/>
-        <v>0.66400000000000003</v>
+        <v>0.73799999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>109</v>
+        <v>89</v>
+      </c>
+      <c r="C31" s="13">
+        <v>39</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>36</v>
@@ -2753,37 +2756,37 @@
         <v>267</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="I31" s="17" t="s">
-        <v>276</v>
+        <v>278</v>
+      </c>
+      <c r="I31" s="15" t="s">
+        <v>279</v>
       </c>
       <c r="J31" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K31">
-        <v>0.123</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="L31" s="6">
         <f t="shared" si="0"/>
-        <v>0.73799999999999999</v>
+        <v>0.182</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C32" s="15">
-        <v>39</v>
+        <v>49</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>36</v>
@@ -2792,37 +2795,37 @@
         <v>267</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="I32" s="17" t="s">
-        <v>279</v>
+        <v>281</v>
+      </c>
+      <c r="I32" s="15" t="s">
+        <v>282</v>
       </c>
       <c r="J32" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="K32">
-        <v>2.5999999999999999E-2</v>
+        <v>0.123</v>
       </c>
       <c r="L32" s="6">
         <f t="shared" si="0"/>
-        <v>0.182</v>
+        <v>0.123</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>48</v>
+        <v>111</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>36</v>
@@ -2831,37 +2834,37 @@
         <v>267</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="I33" s="17" t="s">
-        <v>282</v>
+        <v>285</v>
+      </c>
+      <c r="I33" s="15" t="s">
+        <v>284</v>
       </c>
       <c r="J33" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K33">
-        <v>0.123</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="L33" s="6">
         <f t="shared" si="0"/>
-        <v>0.123</v>
+        <v>0.40200000000000002</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>107</v>
+        <v>93</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>36</v>
@@ -2870,37 +2873,37 @@
         <v>267</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="I34" s="17" t="s">
-        <v>284</v>
+        <v>287</v>
+      </c>
+      <c r="I34" s="15" t="s">
+        <v>288</v>
       </c>
       <c r="J34" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K34">
-        <v>0.20100000000000001</v>
+        <v>2.3E-2</v>
       </c>
       <c r="L34" s="6">
         <f t="shared" si="0"/>
-        <v>0.40200000000000002</v>
+        <v>9.1999999999999998E-2</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>92</v>
+        <v>80</v>
+      </c>
+      <c r="C35" s="13">
+        <v>22</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>36</v>
@@ -2909,37 +2912,37 @@
         <v>267</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="I35" s="17" t="s">
-        <v>288</v>
+        <v>291</v>
+      </c>
+      <c r="I35" s="15" t="s">
+        <v>289</v>
       </c>
       <c r="J35" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K35">
         <v>2.3E-2</v>
       </c>
       <c r="L35" s="6">
         <f t="shared" si="0"/>
-        <v>9.1999999999999998E-2</v>
+        <v>0.161</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" s="15">
-        <v>22</v>
+        <v>37</v>
+      </c>
+      <c r="C36" s="13">
+        <v>0</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>36</v>
@@ -2948,37 +2951,37 @@
         <v>267</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="I36" s="17" t="s">
-        <v>289</v>
+        <v>293</v>
+      </c>
+      <c r="I36" s="15" t="s">
+        <v>294</v>
       </c>
       <c r="J36" s="1">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="K36">
-        <v>2.3E-2</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="L36" s="6">
         <f t="shared" si="0"/>
-        <v>0.161</v>
+        <v>2.1719999999999997</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" s="15">
-        <v>0</v>
+        <v>53</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>36</v>
@@ -2987,37 +2990,37 @@
         <v>267</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="I37" s="17" t="s">
-        <v>294</v>
+        <v>296</v>
+      </c>
+      <c r="I37" s="15" t="s">
+        <v>297</v>
       </c>
       <c r="J37" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="K37">
-        <v>0.18099999999999999</v>
+        <v>2.3E-2</v>
       </c>
       <c r="L37" s="6">
         <f t="shared" si="0"/>
-        <v>2.1719999999999997</v>
+        <v>0.161</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>36</v>
@@ -3026,76 +3029,76 @@
         <v>267</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="I38" s="17" t="s">
-        <v>297</v>
+        <v>299</v>
+      </c>
+      <c r="I38" s="15" t="s">
+        <v>300</v>
       </c>
       <c r="J38" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K38">
-        <v>2.3E-2</v>
+        <v>0.123</v>
       </c>
       <c r="L38" s="6">
         <f t="shared" si="0"/>
-        <v>0.161</v>
+        <v>0.49199999999999999</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>50</v>
+        <v>67</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="I39" s="17" t="s">
-        <v>300</v>
+        <v>302</v>
+      </c>
+      <c r="I39" s="15" t="s">
+        <v>303</v>
       </c>
       <c r="J39" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K39">
-        <v>0.123</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="L39" s="6">
         <f t="shared" si="0"/>
-        <v>0.49199999999999999</v>
+        <v>8.3000000000000004E-2</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>66</v>
+        <v>79</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>78</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>36</v>
@@ -3104,16 +3107,16 @@
         <v>270</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="I40" s="17" t="s">
-        <v>303</v>
+        <v>305</v>
+      </c>
+      <c r="I40" s="15" t="s">
+        <v>306</v>
       </c>
       <c r="J40" s="1">
         <v>1</v>
@@ -3128,13 +3131,13 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>78</v>
+        <v>84</v>
+      </c>
+      <c r="C41" s="13">
+        <v>27</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>36</v>
@@ -3143,16 +3146,16 @@
         <v>270</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="I41" s="17" t="s">
-        <v>306</v>
+        <v>308</v>
+      </c>
+      <c r="I41" s="15" t="s">
+        <v>309</v>
       </c>
       <c r="J41" s="1">
         <v>1</v>
@@ -3167,13 +3170,13 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C42" s="15">
-        <v>27</v>
+        <v>91</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>90</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>36</v>
@@ -3182,16 +3185,16 @@
         <v>270</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="I42" s="17" t="s">
-        <v>309</v>
+        <v>311</v>
+      </c>
+      <c r="I42" s="15" t="s">
+        <v>312</v>
       </c>
       <c r="J42" s="1">
         <v>1</v>
@@ -3206,13 +3209,13 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>90</v>
+        <v>61</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>36</v>
@@ -3221,16 +3224,16 @@
         <v>270</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="I43" s="17" t="s">
-        <v>312</v>
+        <v>314</v>
+      </c>
+      <c r="I43" s="15" t="s">
+        <v>315</v>
       </c>
       <c r="J43" s="1">
         <v>1</v>
@@ -3245,13 +3248,13 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>60</v>
+        <v>108</v>
+      </c>
+      <c r="C44" s="13">
+        <v>100</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>36</v>
@@ -3260,37 +3263,37 @@
         <v>270</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="I44" s="17" t="s">
-        <v>315</v>
+        <v>317</v>
+      </c>
+      <c r="I44" s="15" t="s">
+        <v>284</v>
       </c>
       <c r="J44" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K44">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="L44" s="6">
         <f t="shared" si="0"/>
-        <v>8.3000000000000004E-2</v>
+        <v>0.249</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C45" s="15">
-        <v>100</v>
+        <v>112</v>
+      </c>
+      <c r="C45" s="13">
+        <v>330</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>36</v>
@@ -3299,37 +3302,37 @@
         <v>270</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="I45" s="17" t="s">
-        <v>284</v>
+        <v>319</v>
+      </c>
+      <c r="I45" s="15" t="s">
+        <v>320</v>
       </c>
       <c r="J45" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K45">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="L45" s="6">
         <f t="shared" si="0"/>
-        <v>0.249</v>
+        <v>8.3000000000000004E-2</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C46" s="15">
-        <v>330</v>
+        <v>63</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>36</v>
@@ -3338,132 +3341,132 @@
         <v>270</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="I46" s="17" t="s">
-        <v>320</v>
+        <v>322</v>
+      </c>
+      <c r="I46" s="15" t="s">
+        <v>323</v>
       </c>
       <c r="J46" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K46">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="L46" s="6">
         <f t="shared" si="0"/>
-        <v>8.3000000000000004E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
-        <v>44</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="I47" s="17" t="s">
-        <v>323</v>
-      </c>
-      <c r="J47" s="1">
+        <v>0.16600000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="11">
+        <v>45</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="J47" s="12">
+        <v>1</v>
+      </c>
+      <c r="L47" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="I48" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="J48" s="1">
         <v>2</v>
       </c>
-      <c r="K47">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L47" s="6">
-        <f t="shared" si="0"/>
-        <v>0.16600000000000001</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="13">
-        <v>45</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C48" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D48" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E48" s="1"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="J48" s="14">
-        <v>1</v>
+      <c r="K48">
+        <v>0.29099999999999998</v>
       </c>
       <c r="L48" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.58199999999999996</v>
       </c>
     </row>
     <row r="49" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>46</v>
+      <c r="A49" s="5">
+        <v>16</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>201</v>
+        <v>346</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>198</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>201</v>
+        <v>251</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>327</v>
+        <v>252</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>324</v>
+        <v>254</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="I49" s="17" t="s">
-        <v>326</v>
+        <v>253</v>
+      </c>
+      <c r="I49" s="15" t="s">
+        <v>200</v>
       </c>
       <c r="J49" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K49">
-        <v>0.29099999999999998</v>
+        <v>0.97</v>
       </c>
       <c r="L49" s="6">
-        <f t="shared" si="0"/>
-        <v>0.58199999999999996</v>
+        <f>J49*K49</f>
+        <v>0.97</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -3473,7 +3476,7 @@
       <c r="B50" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C50" s="15" t="s">
+      <c r="C50" s="13" t="s">
         <v>209</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -3491,7 +3494,7 @@
       <c r="H50" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="I50" s="17" t="s">
+      <c r="I50" s="15" t="s">
         <v>328</v>
       </c>
       <c r="J50" s="1">
@@ -3512,7 +3515,7 @@
       <c r="B51" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C51" s="15" t="s">
+      <c r="C51" s="13" t="s">
         <v>204</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -3530,7 +3533,7 @@
       <c r="H51" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="I51" s="17" t="s">
+      <c r="I51" s="15" t="s">
         <v>329</v>
       </c>
       <c r="J51" s="1">
@@ -3551,7 +3554,7 @@
       <c r="B52" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="C52" s="13" t="s">
         <v>120</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -3569,7 +3572,7 @@
       <c r="H52" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="I52" s="17" t="s">
+      <c r="I52" s="15" t="s">
         <v>330</v>
       </c>
       <c r="J52" s="1">
@@ -3590,7 +3593,7 @@
       <c r="B53" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="C53" s="15" t="s">
+      <c r="C53" s="13" t="s">
         <v>188</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -3608,7 +3611,7 @@
       <c r="H53" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="I53" s="17" t="s">
+      <c r="I53" s="15" t="s">
         <v>331</v>
       </c>
       <c r="J53" s="1">
@@ -3629,7 +3632,7 @@
       <c r="B54" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="C54" s="15" t="s">
+      <c r="C54" s="13" t="s">
         <v>212</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -3647,7 +3650,7 @@
       <c r="H54" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="I54" s="17" t="s">
+      <c r="I54" s="15" t="s">
         <v>212</v>
       </c>
       <c r="J54" s="1">
@@ -3668,7 +3671,7 @@
       <c r="B55" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="C55" s="15" t="s">
+      <c r="C55" s="13" t="s">
         <v>184</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -3686,7 +3689,7 @@
       <c r="H55" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I55" s="17" t="s">
+      <c r="I55" s="15" t="s">
         <v>17</v>
       </c>
       <c r="J55" s="1">
@@ -3707,7 +3710,7 @@
       <c r="B56" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C56" s="15" t="s">
+      <c r="C56" s="13" t="s">
         <v>157</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -3725,7 +3728,7 @@
       <c r="H56" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="I56" s="17" t="s">
+      <c r="I56" s="15" t="s">
         <v>332</v>
       </c>
       <c r="J56" s="1">
@@ -3746,7 +3749,7 @@
       <c r="B57" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="15" t="s">
+      <c r="C57" s="13" t="s">
         <v>101</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -3764,7 +3767,7 @@
       <c r="H57" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="I57" s="17" t="s">
+      <c r="I57" s="15" t="s">
         <v>333</v>
       </c>
       <c r="J57" s="1">
@@ -3785,7 +3788,7 @@
       <c r="B58" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="C58" s="13" t="s">
         <v>163</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -3803,7 +3806,7 @@
       <c r="H58" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="I58" s="17" t="s">
+      <c r="I58" s="15" t="s">
         <v>334</v>
       </c>
       <c r="J58" s="1">
@@ -3824,7 +3827,7 @@
       <c r="B59" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C59" s="15" t="s">
+      <c r="C59" s="13" t="s">
         <v>179</v>
       </c>
       <c r="D59" s="1" t="s">
@@ -3842,7 +3845,7 @@
       <c r="H59" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="I59" s="17" t="s">
+      <c r="I59" s="15" t="s">
         <v>335</v>
       </c>
       <c r="J59" s="1">
@@ -3863,7 +3866,7 @@
       <c r="B60" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C60" s="15" t="s">
+      <c r="C60" s="13" t="s">
         <v>169</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -3881,7 +3884,7 @@
       <c r="H60" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="I60" s="17" t="s">
+      <c r="I60" s="15" t="s">
         <v>336</v>
       </c>
       <c r="J60" s="1">
@@ -3902,7 +3905,7 @@
       <c r="B61" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C61" s="15" t="s">
+      <c r="C61" s="13" t="s">
         <v>124</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -3920,7 +3923,7 @@
       <c r="H61" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="I61" s="17" t="s">
+      <c r="I61" s="15" t="s">
         <v>337</v>
       </c>
       <c r="J61" s="1">
@@ -3941,7 +3944,7 @@
       <c r="B62" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C62" s="15" t="s">
+      <c r="C62" s="13" t="s">
         <v>174</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -3959,7 +3962,7 @@
       <c r="H62" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="I62" s="17" t="s">
+      <c r="I62" s="15" t="s">
         <v>338</v>
       </c>
       <c r="J62" s="1">
@@ -3980,7 +3983,7 @@
       <c r="B63" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="C63" s="15" t="s">
+      <c r="C63" s="13" t="s">
         <v>20</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -3998,7 +4001,7 @@
       <c r="H63" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="I63" s="17" t="s">
+      <c r="I63" s="15" t="s">
         <v>339</v>
       </c>
       <c r="J63" s="1">
@@ -4032,7 +4035,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.140625" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" style="8" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" customWidth="1"/>
     <col min="5" max="5" width="43.85546875" bestFit="1" customWidth="1"/>
@@ -4043,35 +4046,35 @@
     <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="9" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4079,7 +4082,7 @@
       <c r="A2" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C2" t="s">
@@ -4105,7 +4108,7 @@
       <c r="A3" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>113</v>
       </c>
       <c r="C3" t="s">
@@ -4131,7 +4134,7 @@
       <c r="A4" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>58</v>
       </c>
       <c r="C4" t="s">
@@ -4148,7 +4151,7 @@
       <c r="A5" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C5" t="s">
@@ -4165,7 +4168,7 @@
       <c r="A6" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>76</v>
       </c>
       <c r="C6" t="s">
@@ -4182,7 +4185,7 @@
       <c r="A7" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>42</v>
       </c>
       <c r="C7" t="s">
@@ -4199,7 +4202,7 @@
       <c r="A8" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>74</v>
       </c>
       <c r="C8" t="s">
@@ -4216,7 +4219,7 @@
       <c r="A9" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>68</v>
       </c>
       <c r="C9" t="s">
@@ -4233,7 +4236,7 @@
       <c r="A10" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>54</v>
       </c>
       <c r="C10" t="s">
@@ -4256,7 +4259,7 @@
       <c r="A11" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="8" t="s">
         <v>46</v>
       </c>
       <c r="C11" t="s">
@@ -4290,7 +4293,7 @@
       <c r="A13" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="8" t="s">
         <v>81</v>
       </c>
       <c r="C13" t="s">
@@ -4307,7 +4310,7 @@
       <c r="A14" t="s">
         <v>119</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="8" t="s">
         <v>118</v>
       </c>
       <c r="C14" t="s">
@@ -4324,7 +4327,7 @@
       <c r="A15" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="8" t="s">
         <v>72</v>
       </c>
       <c r="C15" t="s">
@@ -4341,7 +4344,7 @@
       <c r="A16" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="8" t="s">
         <v>64</v>
       </c>
       <c r="C16" t="s">
@@ -4358,7 +4361,7 @@
       <c r="A17" t="s">
         <v>199</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="8" t="s">
         <v>198</v>
       </c>
       <c r="C17" t="s">
@@ -4375,7 +4378,7 @@
       <c r="A18" t="s">
         <v>147</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="8" t="s">
         <v>146</v>
       </c>
       <c r="C18" t="s">
@@ -4401,7 +4404,7 @@
       <c r="A19" t="s">
         <v>141</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="8" t="s">
         <v>140</v>
       </c>
       <c r="C19" t="s">
@@ -4427,7 +4430,7 @@
       <c r="A20" t="s">
         <v>131</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="8" t="s">
         <v>130</v>
       </c>
       <c r="C20" t="s">
@@ -4453,7 +4456,7 @@
       <c r="A21" t="s">
         <v>137</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="8" t="s">
         <v>136</v>
       </c>
       <c r="C21" t="s">
@@ -4479,7 +4482,7 @@
       <c r="A22" t="s">
         <v>153</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="8" t="s">
         <v>152</v>
       </c>
       <c r="C22" t="s">
@@ -4505,7 +4508,7 @@
       <c r="A23" t="s">
         <v>87</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="8" t="s">
         <v>85</v>
       </c>
       <c r="C23" t="s">
@@ -4562,7 +4565,7 @@
       <c r="A26" t="s">
         <v>194</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="8" t="s">
         <v>193</v>
       </c>
       <c r="C26" t="s">
@@ -4579,7 +4582,7 @@
       <c r="A27" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="8" t="s">
         <v>70</v>
       </c>
       <c r="C27" t="s">
@@ -4596,7 +4599,7 @@
       <c r="A28" t="s">
         <v>83</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="8">
         <v>24.9</v>
       </c>
       <c r="C28" t="s">
@@ -4613,7 +4616,7 @@
       <c r="A29" t="s">
         <v>110</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="8" t="s">
         <v>109</v>
       </c>
       <c r="C29" t="s">
@@ -4630,7 +4633,7 @@
       <c r="A30" t="s">
         <v>89</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B30" s="8">
         <v>39</v>
       </c>
       <c r="C30" t="s">
@@ -4647,7 +4650,7 @@
       <c r="A31" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="8" t="s">
         <v>48</v>
       </c>
       <c r="C31" t="s">
@@ -4664,7 +4667,7 @@
       <c r="A32" t="s">
         <v>111</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B32" s="8">
         <v>110</v>
       </c>
       <c r="C32" t="s">
@@ -4681,7 +4684,7 @@
       <c r="A33" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B33" s="8">
         <v>49.9</v>
       </c>
       <c r="C33" t="s">
@@ -4698,7 +4701,7 @@
       <c r="A34" t="s">
         <v>80</v>
       </c>
-      <c r="B34" s="10">
+      <c r="B34" s="8">
         <v>22</v>
       </c>
       <c r="C34" t="s">
@@ -4715,7 +4718,7 @@
       <c r="A35" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="10">
+      <c r="B35" s="8">
         <v>0</v>
       </c>
       <c r="C35" t="s">
@@ -4732,7 +4735,7 @@
       <c r="A36" t="s">
         <v>53</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C36" t="s">
@@ -4749,7 +4752,7 @@
       <c r="A37" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="8" t="s">
         <v>50</v>
       </c>
       <c r="C37" t="s">
@@ -4766,7 +4769,7 @@
       <c r="A38" t="s">
         <v>67</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="8" t="s">
         <v>66</v>
       </c>
       <c r="C38" t="s">
@@ -4783,7 +4786,7 @@
       <c r="A39" t="s">
         <v>79</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C39" t="s">
@@ -4800,7 +4803,7 @@
       <c r="A40" t="s">
         <v>84</v>
       </c>
-      <c r="B40" s="10">
+      <c r="B40" s="8">
         <v>27</v>
       </c>
       <c r="C40" t="s">
@@ -4817,7 +4820,7 @@
       <c r="A41" t="s">
         <v>91</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="8" t="s">
         <v>90</v>
       </c>
       <c r="C41" t="s">
@@ -4834,7 +4837,7 @@
       <c r="A42" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="8" t="s">
         <v>60</v>
       </c>
       <c r="C42" t="s">
@@ -4851,7 +4854,7 @@
       <c r="A43" t="s">
         <v>108</v>
       </c>
-      <c r="B43" s="10">
+      <c r="B43" s="8">
         <v>100</v>
       </c>
       <c r="C43" t="s">
@@ -4868,7 +4871,7 @@
       <c r="A44" t="s">
         <v>112</v>
       </c>
-      <c r="B44" s="10">
+      <c r="B44" s="8">
         <v>330</v>
       </c>
       <c r="C44" t="s">
@@ -4885,7 +4888,7 @@
       <c r="A45" t="s">
         <v>63</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="8" t="s">
         <v>62</v>
       </c>
       <c r="C45" t="s">
@@ -4902,7 +4905,7 @@
       <c r="A46" t="s">
         <v>40</v>
       </c>
-      <c r="B46" s="10">
+      <c r="B46" s="8">
         <v>0</v>
       </c>
       <c r="C46" t="s">
@@ -4922,7 +4925,7 @@
       <c r="A47" t="s">
         <v>202</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="8" t="s">
         <v>201</v>
       </c>
       <c r="C47" t="s">
@@ -4939,7 +4942,7 @@
       <c r="A48" t="s">
         <v>210</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="8" t="s">
         <v>209</v>
       </c>
       <c r="C48" t="s">
@@ -4965,7 +4968,7 @@
       <c r="A49" t="s">
         <v>205</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="8" t="s">
         <v>204</v>
       </c>
       <c r="C49" t="s">
@@ -4991,7 +4994,7 @@
       <c r="A50" t="s">
         <v>12</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B50" s="8" t="s">
         <v>120</v>
       </c>
       <c r="C50" t="s">
@@ -5017,7 +5020,7 @@
       <c r="A51" t="s">
         <v>189</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B51" s="8" t="s">
         <v>188</v>
       </c>
       <c r="C51" t="s">
@@ -5043,7 +5046,7 @@
       <c r="A52" t="s">
         <v>213</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="B52" s="8" t="s">
         <v>212</v>
       </c>
       <c r="C52" t="s">
@@ -5069,7 +5072,7 @@
       <c r="A53" t="s">
         <v>185</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="B53" s="8" t="s">
         <v>184</v>
       </c>
       <c r="C53" t="s">
@@ -5098,7 +5101,7 @@
       <c r="A54" t="s">
         <v>158</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="B54" s="8" t="s">
         <v>157</v>
       </c>
       <c r="C54" t="s">
@@ -5124,7 +5127,7 @@
       <c r="A55" t="s">
         <v>102</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="B55" s="8" t="s">
         <v>101</v>
       </c>
       <c r="C55" t="s">
@@ -5150,7 +5153,7 @@
       <c r="A56" t="s">
         <v>164</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="B56" s="8" t="s">
         <v>163</v>
       </c>
       <c r="C56" t="s">
@@ -5176,7 +5179,7 @@
       <c r="A57" t="s">
         <v>180</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="B57" s="8" t="s">
         <v>179</v>
       </c>
       <c r="C57" t="s">
@@ -5202,7 +5205,7 @@
       <c r="A58" t="s">
         <v>170</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B58" s="8" t="s">
         <v>169</v>
       </c>
       <c r="C58" t="s">
@@ -5228,7 +5231,7 @@
       <c r="A59" t="s">
         <v>125</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B59" s="8" t="s">
         <v>124</v>
       </c>
       <c r="C59" t="s">
@@ -5254,7 +5257,7 @@
       <c r="A60" t="s">
         <v>175</v>
       </c>
-      <c r="B60" s="10" t="s">
+      <c r="B60" s="8" t="s">
         <v>174</v>
       </c>
       <c r="C60" t="s">
@@ -5280,7 +5283,7 @@
       <c r="A61" t="s">
         <v>217</v>
       </c>
-      <c r="B61" s="10" t="s">
+      <c r="B61" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C61" t="s">

</xml_diff>

<commit_message>
Finalized BOM and re-exported all assembly, CAM and prevue files.
</commit_message>
<xml_diff>
--- a/hardware/MainBoard/MainBoard_BOM.xlsx
+++ b/hardware/MainBoard/MainBoard_BOM.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="346">
   <si>
     <t>Item #</t>
   </si>
@@ -712,12 +712,6 @@
     <t>Standoff</t>
   </si>
   <si>
-    <t>C1005X5R0G225M</t>
-  </si>
-  <si>
-    <t>445-3882-1-ND</t>
-  </si>
-  <si>
     <t>TDK</t>
   </si>
   <si>
@@ -730,18 +724,12 @@
     <t>CAP CER 0.1UF 16V 10% X7R 0402</t>
   </si>
   <si>
-    <t>CAP CER 2.2UF 4V 20% X5R 0402</t>
-  </si>
-  <si>
     <t>FILTER CHIP 600 OHM 500MA 0603</t>
   </si>
   <si>
     <t>FERRITE CHIP 70 OHM 4000MA 0603</t>
   </si>
   <si>
-    <t>Use 4.7uF instead?</t>
-  </si>
-  <si>
     <t>C1005X7R1C103M</t>
   </si>
   <si>
@@ -769,21 +757,6 @@
     <t>CAP CER 4PF 50V NP0 0402</t>
   </si>
   <si>
-    <t>Device number corresponds to 0603 footprint</t>
-  </si>
-  <si>
-    <t>&lt;10 V rated, is it sufficient?</t>
-  </si>
-  <si>
-    <t>C1005X5R0J334K</t>
-  </si>
-  <si>
-    <t>445-4994-1-ND</t>
-  </si>
-  <si>
-    <t>CAP CER 0.33UF 6.3V 10% X5R 0402</t>
-  </si>
-  <si>
     <t>C1005C0G1H220J</t>
   </si>
   <si>
@@ -1093,17 +1066,41 @@
     <t>M8487CT-ND</t>
   </si>
   <si>
-    <t>Out of stock at digi-key, do we have it in house? Should we go Mouser?</t>
-  </si>
-  <si>
     <t>SW3</t>
+  </si>
+  <si>
+    <t>C27, C49, C50, C51, C123, C127, C129, C136, C138, C140, C142</t>
+  </si>
+  <si>
+    <t>Taiyo Yuden</t>
+  </si>
+  <si>
+    <t>LMK105BJ225MV-F</t>
+  </si>
+  <si>
+    <t>587-3153-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 2.2UF 10V 20% X5R 0402</t>
+  </si>
+  <si>
+    <t>C1, C40, C70, C72, C74, C76, C78, C80, C82, C84, C100, C102, C104, C106, C108, C110, C112, C114</t>
+  </si>
+  <si>
+    <t>C1005X5R1C334K</t>
+  </si>
+  <si>
+    <t>445-4974-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 0.33UF 16V 10% X5R 0402</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1150,15 +1147,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1170,13 +1160,8 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1238,29 +1223,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1302,16 +1271,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1319,8 +1278,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+  <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
@@ -1626,17 +1584,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M63"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="27" style="1" customWidth="1"/>
     <col min="5" max="5" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" style="1" bestFit="1" customWidth="1"/>
@@ -1649,23 +1607,23 @@
     <col min="13" max="13" width="43.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -1703,7 +1661,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -1729,7 +1687,7 @@
         <v>98</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="J4" s="1">
         <v>1</v>
@@ -1742,7 +1700,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -1768,7 +1726,7 @@
         <v>116</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="J5" s="1">
         <v>3</v>
@@ -1777,16 +1735,16 @@
         <v>0.38</v>
       </c>
       <c r="L5" s="6">
-        <f t="shared" ref="L5:L63" si="0">J5*K5</f>
+        <f t="shared" ref="L5:L61" si="0">J5*K5</f>
         <v>1.1400000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>59</v>
+        <v>342</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>58</v>
@@ -1795,35 +1753,32 @@
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>218</v>
+        <v>338</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>339</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>224</v>
+        <v>340</v>
+      </c>
+      <c r="I6" t="s">
+        <v>341</v>
       </c>
       <c r="J6" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K6">
         <v>0.3</v>
       </c>
       <c r="L6" s="6">
         <f t="shared" si="0"/>
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="M6" s="19" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>5.3999999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>4</v>
       </c>
@@ -1837,19 +1792,19 @@
         <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="I7" s="15" t="s">
         <v>221</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>223</v>
       </c>
       <c r="J7" s="1">
         <v>73</v>
@@ -1862,1066 +1817,1072 @@
         <v>6.5699999999999994</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="H8" s="1" t="s">
+        <v>225</v>
+      </c>
       <c r="I8" s="15" t="s">
-        <v>26</v>
+        <v>226</v>
       </c>
       <c r="J8" s="1">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="K8">
+        <v>0.08</v>
       </c>
       <c r="L8" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M8" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="I9" s="15" t="s">
-        <v>230</v>
-      </c>
       <c r="J9" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K9">
         <v>0.08</v>
       </c>
       <c r="L9" s="6">
         <f t="shared" si="0"/>
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="I10" s="15" t="s">
-        <v>233</v>
-      </c>
       <c r="J10" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K10">
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="L10" s="6">
         <f t="shared" si="0"/>
-        <v>0.32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>234</v>
+        <v>343</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>236</v>
+        <v>344</v>
+      </c>
+      <c r="I11" t="s">
+        <v>345</v>
       </c>
       <c r="J11" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K11">
-        <v>0.2</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="L11" s="6">
         <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+        <v>1.9600000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
         <v>9</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="17" t="s">
+      <c r="B12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I12" s="15" t="s">
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="1">
-        <v>1</v>
+      <c r="J12" s="12">
+        <v>18</v>
       </c>
       <c r="L12" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M12" s="19" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+    </row>
+    <row r="13" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
         <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="J13" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K13">
-        <v>0.28000000000000003</v>
+        <v>0.08</v>
       </c>
       <c r="L13" s="6">
         <f t="shared" si="0"/>
-        <v>1.9600000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
-        <v>11</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="12" t="s">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14" s="12">
-        <v>18</v>
+      <c r="E14" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="J14" s="1">
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <v>0.08</v>
       </c>
       <c r="L14" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="G15" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="J15" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="K15">
         <v>0.08</v>
       </c>
       <c r="L15" s="6">
         <f t="shared" si="0"/>
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>119</v>
+        <v>337</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>118</v>
+        <v>64</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="J16" s="1">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="K16">
-        <v>0.08</v>
+        <v>0.53</v>
       </c>
       <c r="L16" s="6">
         <f t="shared" si="0"/>
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+        <v>5.83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
         <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>73</v>
+        <v>199</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>72</v>
+        <v>152</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>24</v>
+        <v>152</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>220</v>
+        <v>156</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="G17" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>229</v>
+        <v>155</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="J17" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K17">
-        <v>0.08</v>
+        <v>1.6</v>
       </c>
       <c r="L17" s="6">
-        <f t="shared" si="0"/>
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <f>J17*K17</f>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>65</v>
+        <v>147</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>64</v>
+        <v>146</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>24</v>
+        <v>146</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="J18" s="1">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="L18" s="6">
+        <f t="shared" si="0"/>
+        <v>8.2100000000000009</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>16</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I19" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="I18" s="15" t="s">
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>3.45</v>
+      </c>
+      <c r="L19" s="6">
+        <f t="shared" si="0"/>
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>17</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="J20" s="1">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>5.81</v>
+      </c>
+      <c r="L20" s="6">
+        <f t="shared" si="0"/>
+        <v>5.81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>18</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I21" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="J18" s="1">
-        <v>4</v>
-      </c>
-      <c r="K18">
-        <v>0.53</v>
-      </c>
-      <c r="L18" s="6">
-        <f t="shared" si="0"/>
-        <v>2.12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>21</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="I19" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="J19" s="1">
-        <v>1</v>
-      </c>
-      <c r="K19">
-        <v>1.6</v>
-      </c>
-      <c r="L19" s="6">
-        <f>J19*K19</f>
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
-        <v>17</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="I20" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="J20" s="1">
-        <v>1</v>
-      </c>
-      <c r="K20">
-        <v>8.2100000000000009</v>
-      </c>
-      <c r="L20" s="6">
-        <f t="shared" si="0"/>
-        <v>8.2100000000000009</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>18</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="I21" s="15" t="s">
-        <v>257</v>
-      </c>
       <c r="J21" s="1">
         <v>1</v>
       </c>
       <c r="K21">
-        <v>3.45</v>
+        <v>6.24</v>
       </c>
       <c r="L21" s="6">
         <f t="shared" si="0"/>
-        <v>3.45</v>
-      </c>
-      <c r="M21" s="19" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>6.24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>19</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>131</v>
+        <v>87</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>130</v>
+        <v>85</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>134</v>
+        <v>334</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="G22" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>133</v>
+        <v>335</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>256</v>
+        <v>332</v>
       </c>
       <c r="J22" s="1">
-        <v>1</v>
-      </c>
-      <c r="K22">
-        <v>5.81</v>
+        <v>2</v>
       </c>
       <c r="L22" s="6">
         <f t="shared" si="0"/>
-        <v>5.81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>20</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>136</v>
+        <v>34</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>136</v>
+        <v>33</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>134</v>
+        <v>31</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G23" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>138</v>
+        <v>250</v>
       </c>
       <c r="I23" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>0.6</v>
+      </c>
+      <c r="L23" s="6">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>21</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>0.33</v>
+      </c>
+      <c r="L24" s="6">
+        <f t="shared" si="0"/>
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>22</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="J25" s="1">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>0.37</v>
+      </c>
+      <c r="L25" s="6">
+        <f t="shared" si="0"/>
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>23</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="J23" s="1">
-        <v>1</v>
-      </c>
-      <c r="K23">
-        <v>6.24</v>
-      </c>
-      <c r="L23" s="6">
-        <f t="shared" si="0"/>
-        <v>6.24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>22</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="I24" s="15" t="s">
-        <v>341</v>
-      </c>
-      <c r="J24" s="1">
-        <v>2</v>
-      </c>
-      <c r="L24" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
-        <v>23</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H25" s="1" t="s">
+      <c r="F26" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="I25" s="15" t="s">
+      <c r="I26" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="J25" s="1">
-        <v>1</v>
-      </c>
-      <c r="K25">
-        <v>0.6</v>
-      </c>
-      <c r="L25" s="6">
-        <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="J26" s="1">
+        <v>6</v>
+      </c>
+      <c r="K26">
+        <v>2.3E-2</v>
+      </c>
+      <c r="L26" s="6">
+        <f t="shared" si="0"/>
+        <v>0.13800000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
         <v>24</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H26" s="1" t="s">
+      <c r="B27" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="13">
+        <v>24.9</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="I26" s="15" t="s">
+      <c r="F27" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="J26" s="1">
-        <v>1</v>
-      </c>
-      <c r="K26">
-        <v>0.33</v>
-      </c>
-      <c r="L26" s="6">
-        <f t="shared" si="0"/>
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="G27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="I27" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="J27" s="1">
+        <v>8</v>
+      </c>
+      <c r="K27">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L27" s="6">
+        <f t="shared" si="0"/>
+        <v>0.66400000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
         <v>25</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="I27" s="15" t="s">
-        <v>265</v>
-      </c>
-      <c r="J27" s="1">
-        <v>1</v>
-      </c>
-      <c r="K27">
-        <v>0.37</v>
-      </c>
-      <c r="L27" s="6">
-        <f t="shared" si="0"/>
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
-        <v>26</v>
-      </c>
       <c r="B28" s="3" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="I28" s="15" t="s">
         <v>267</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="I28" s="15" t="s">
-        <v>269</v>
       </c>
       <c r="J28" s="1">
         <v>6</v>
       </c>
       <c r="K28">
-        <v>2.3E-2</v>
+        <v>0.123</v>
       </c>
       <c r="L28" s="6">
         <f t="shared" si="0"/>
-        <v>0.13800000000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>27</v>
+        <v>0.73799999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>26</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C29" s="13">
-        <v>24.9</v>
+        <v>39</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="I29" s="15" t="s">
         <v>270</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="I29" s="15" t="s">
-        <v>273</v>
-      </c>
       <c r="J29" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K29">
-        <v>8.3000000000000004E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="L29" s="6">
         <f t="shared" si="0"/>
-        <v>0.66400000000000003</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.182</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>110</v>
+        <v>49</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>109</v>
+        <v>48</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="J30" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K30">
         <v>0.123</v>
       </c>
       <c r="L30" s="6">
         <f t="shared" si="0"/>
-        <v>0.73799999999999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C31" s="13">
-        <v>39</v>
+        <v>111</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="I31" s="15" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="J31" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K31">
-        <v>2.5999999999999999E-2</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="L31" s="6">
         <f t="shared" si="0"/>
-        <v>0.182</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.40200000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J32" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K32">
-        <v>0.123</v>
+        <v>2.3E-2</v>
       </c>
       <c r="L32" s="6">
         <f t="shared" si="0"/>
-        <v>0.123</v>
+        <v>9.1999999999999998E-2</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
-        <v>31</v>
+      <c r="A33" s="5">
+        <v>30</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>107</v>
+        <v>80</v>
+      </c>
+      <c r="C33" s="13">
+        <v>22</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I33" s="15" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="J33" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K33">
-        <v>0.20100000000000001</v>
+        <v>2.3E-2</v>
       </c>
       <c r="L33" s="6">
         <f t="shared" si="0"/>
-        <v>0.40200000000000002</v>
+        <v>0.161</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>92</v>
+        <v>37</v>
+      </c>
+      <c r="C34" s="13">
+        <v>0</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="J34" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="K34">
-        <v>2.3E-2</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="L34" s="6">
         <f t="shared" si="0"/>
-        <v>9.1999999999999998E-2</v>
+        <v>2.1719999999999997</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C35" s="13">
-        <v>22</v>
+        <v>53</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="I35" s="15" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J35" s="1">
         <v>7</v>
@@ -2936,148 +2897,148 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="13">
-        <v>0</v>
+        <v>51</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="I36" s="15" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="J36" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="K36">
-        <v>0.18099999999999999</v>
+        <v>0.123</v>
       </c>
       <c r="L36" s="6">
         <f t="shared" si="0"/>
-        <v>2.1719999999999997</v>
+        <v>0.49199999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
-        <v>35</v>
+      <c r="A37" s="5">
+        <v>34</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="J37" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="K37">
-        <v>2.3E-2</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="L37" s="6">
         <f t="shared" si="0"/>
-        <v>0.161</v>
+        <v>8.3000000000000004E-2</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="J38" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K38">
-        <v>0.123</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="L38" s="6">
         <f t="shared" si="0"/>
-        <v>0.49199999999999999</v>
+        <v>8.3000000000000004E-2</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>66</v>
+        <v>84</v>
+      </c>
+      <c r="C39" s="13">
+        <v>27</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I39" s="15" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="J39" s="1">
         <v>1</v>
@@ -3092,31 +3053,31 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="I40" s="15" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="J40" s="1">
         <v>1</v>
@@ -3130,32 +3091,32 @@
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
-        <v>39</v>
+      <c r="A41" s="5">
+        <v>38</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C41" s="13">
-        <v>27</v>
+        <v>61</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="I41" s="15" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="J41" s="1">
         <v>1</v>
@@ -3170,70 +3131,70 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>90</v>
+        <v>108</v>
+      </c>
+      <c r="C42" s="13">
+        <v>100</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="I42" s="15" t="s">
-        <v>312</v>
+        <v>275</v>
       </c>
       <c r="J42" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K42">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="L42" s="6">
         <f t="shared" si="0"/>
-        <v>8.3000000000000004E-2</v>
+        <v>0.249</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>60</v>
+        <v>112</v>
+      </c>
+      <c r="C43" s="13">
+        <v>330</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="I43" s="15" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="J43" s="1">
         <v>1</v>
@@ -3248,225 +3209,225 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C44" s="13">
-        <v>100</v>
+        <v>63</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="I44" s="15" t="s">
-        <v>284</v>
+        <v>314</v>
       </c>
       <c r="J44" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K44">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="L44" s="6">
         <f t="shared" si="0"/>
-        <v>0.249</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
+        <v>0.16600000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="11">
+        <v>42</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="J45" s="12">
+        <v>1</v>
+      </c>
+      <c r="L45" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
         <v>43</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C45" s="13">
-        <v>330</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="F45" s="1" t="s">
+      <c r="B46" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="G45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="I45" s="15" t="s">
-        <v>320</v>
-      </c>
-      <c r="J45" s="1">
-        <v>1</v>
-      </c>
-      <c r="K45">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L45" s="6">
-        <f t="shared" si="0"/>
-        <v>8.3000000000000004E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
-        <v>44</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>270</v>
-      </c>
       <c r="F46" s="1" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="I46" s="15" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="J46" s="1">
         <v>2</v>
       </c>
       <c r="K46">
-        <v>8.3000000000000004E-2</v>
+        <v>0.29099999999999998</v>
       </c>
       <c r="L46" s="6">
         <f t="shared" si="0"/>
-        <v>0.16600000000000001</v>
+        <v>0.58199999999999996</v>
       </c>
     </row>
     <row r="47" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="11">
+      <c r="A47" s="4">
+        <v>44</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="I47" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="J47" s="1">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>0.97</v>
+      </c>
+      <c r="L47" s="6">
+        <f>J47*K47</f>
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
         <v>45</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D47" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E47" s="1"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="12"/>
-      <c r="I47" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="J47" s="12">
-        <v>1</v>
-      </c>
-      <c r="L47" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>46</v>
-      </c>
       <c r="B48" s="3" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="G48" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F48" s="1">
+        <v>5009</v>
+      </c>
+      <c r="G48" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>325</v>
+        <v>211</v>
       </c>
       <c r="I48" s="15" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="J48" s="1">
         <v>2</v>
       </c>
       <c r="K48">
-        <v>0.29099999999999998</v>
+        <v>0.35</v>
       </c>
       <c r="L48" s="6">
         <f t="shared" si="0"/>
-        <v>0.58199999999999996</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>346</v>
+        <v>205</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>251</v>
+        <v>204</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="G49" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F49" s="1">
+        <v>5121</v>
+      </c>
+      <c r="G49" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>253</v>
+        <v>207</v>
       </c>
       <c r="I49" s="15" t="s">
-        <v>200</v>
+        <v>320</v>
       </c>
       <c r="J49" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K49">
-        <v>0.97</v>
+        <v>0.35</v>
       </c>
       <c r="L49" s="6">
-        <f>J49*K49</f>
-        <v>0.97</v>
+        <f t="shared" si="0"/>
+        <v>0.7</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -3474,38 +3435,38 @@
         <v>47</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>209</v>
+        <v>120</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>209</v>
+        <v>120</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="F50" s="1">
-        <v>5009</v>
+        <v>123</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>211</v>
+        <v>122</v>
       </c>
       <c r="I50" s="15" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="J50" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K50">
-        <v>0.35</v>
+        <v>53.91</v>
       </c>
       <c r="L50" s="6">
         <f t="shared" si="0"/>
-        <v>0.7</v>
+        <v>53.91</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -3513,38 +3474,38 @@
         <v>48</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="F51" s="1">
-        <v>5121</v>
+        <v>167</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="I51" s="15" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="J51" s="1">
         <v>2</v>
       </c>
       <c r="K51">
-        <v>0.35</v>
+        <v>20.09</v>
       </c>
       <c r="L51" s="6">
         <f t="shared" si="0"/>
-        <v>0.7</v>
+        <v>40.18</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -3552,77 +3513,77 @@
         <v>49</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>12</v>
+        <v>213</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>120</v>
+        <v>212</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>120</v>
+        <v>212</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>123</v>
+        <v>216</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>120</v>
+        <v>212</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>122</v>
+        <v>215</v>
       </c>
       <c r="I52" s="15" t="s">
-        <v>330</v>
+        <v>212</v>
       </c>
       <c r="J52" s="1">
         <v>1</v>
       </c>
       <c r="K52">
-        <v>53.91</v>
+        <v>0.95</v>
       </c>
       <c r="L52" s="6">
         <f t="shared" si="0"/>
-        <v>53.91</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
+      <c r="A53" s="5">
         <v>50</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>167</v>
+        <v>16</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>192</v>
+        <v>15</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>191</v>
+        <v>15</v>
       </c>
       <c r="I53" s="15" t="s">
-        <v>331</v>
+        <v>17</v>
       </c>
       <c r="J53" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K53">
-        <v>20.09</v>
+        <v>4.25</v>
       </c>
       <c r="L53" s="6">
         <f t="shared" si="0"/>
-        <v>40.18</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -3630,38 +3591,38 @@
         <v>51</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>213</v>
+        <v>158</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>212</v>
+        <v>157</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>212</v>
+        <v>157</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>216</v>
+        <v>161</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>212</v>
+        <v>162</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>215</v>
+        <v>160</v>
       </c>
       <c r="I54" s="15" t="s">
-        <v>212</v>
+        <v>323</v>
       </c>
       <c r="J54" s="1">
         <v>1</v>
       </c>
       <c r="K54">
-        <v>0.95</v>
+        <v>6.66</v>
       </c>
       <c r="L54" s="6">
         <f t="shared" si="0"/>
-        <v>0.95</v>
+        <v>6.66</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -3669,348 +3630,270 @@
         <v>52</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>185</v>
+        <v>102</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>184</v>
+        <v>101</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>184</v>
+        <v>101</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>16</v>
+        <v>105</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>15</v>
+        <v>106</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>15</v>
+        <v>104</v>
       </c>
       <c r="I55" s="15" t="s">
-        <v>17</v>
+        <v>324</v>
       </c>
       <c r="J55" s="1">
         <v>1</v>
       </c>
       <c r="K55">
-        <v>4.25</v>
+        <v>0.34</v>
       </c>
       <c r="L55" s="6">
         <f t="shared" si="0"/>
-        <v>4.25</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>53</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="I56" s="15" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="J56" s="1">
         <v>1</v>
       </c>
       <c r="K56">
-        <v>6.66</v>
+        <v>0.81</v>
       </c>
       <c r="L56" s="6">
         <f t="shared" si="0"/>
-        <v>6.66</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="4">
+      <c r="A57" s="5">
         <v>54</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>102</v>
+        <v>180</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>101</v>
+        <v>179</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>101</v>
+        <v>179</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>105</v>
+        <v>172</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>106</v>
+        <v>183</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>104</v>
+        <v>182</v>
       </c>
       <c r="I57" s="15" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="J57" s="1">
         <v>1</v>
       </c>
       <c r="K57">
-        <v>0.34</v>
+        <v>4.3099999999999996</v>
       </c>
       <c r="L57" s="6">
         <f t="shared" si="0"/>
-        <v>0.34</v>
+        <v>4.3099999999999996</v>
       </c>
     </row>
     <row r="58" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="5">
+      <c r="A58" s="4">
         <v>55</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="I58" s="15" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="J58" s="1">
         <v>1</v>
       </c>
       <c r="K58">
-        <v>0.81</v>
+        <v>1.58</v>
       </c>
       <c r="L58" s="6">
         <f t="shared" si="0"/>
-        <v>0.81</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="5">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
         <v>56</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>180</v>
+        <v>125</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>179</v>
+        <v>124</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>179</v>
+        <v>124</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>172</v>
+        <v>128</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>183</v>
+        <v>129</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>182</v>
+        <v>127</v>
       </c>
       <c r="I59" s="15" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="J59" s="1">
         <v>1</v>
       </c>
       <c r="K59">
-        <v>4.3099999999999996</v>
+        <v>2.59</v>
       </c>
       <c r="L59" s="6">
         <f t="shared" si="0"/>
-        <v>4.3099999999999996</v>
+        <v>2.59</v>
       </c>
     </row>
     <row r="60" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="5">
+      <c r="A60" s="4">
         <v>57</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>172</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="I60" s="15" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="J60" s="1">
         <v>1</v>
       </c>
       <c r="K60">
-        <v>1.58</v>
+        <v>2.06</v>
       </c>
       <c r="L60" s="6">
         <f t="shared" si="0"/>
-        <v>1.58</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>2.06</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>58</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>125</v>
+        <v>217</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>124</v>
+        <v>20</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>124</v>
+        <v>196</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G61" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F61" s="1">
+        <v>7200</v>
+      </c>
+      <c r="G61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>127</v>
+        <v>331</v>
       </c>
       <c r="I61" s="15" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="J61" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K61">
-        <v>2.59</v>
+        <v>0.68</v>
       </c>
       <c r="L61" s="6">
-        <f t="shared" si="0"/>
-        <v>2.59</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4">
-        <v>59</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C62" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="G62" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="I62" s="15" t="s">
-        <v>338</v>
-      </c>
-      <c r="J62" s="1">
-        <v>1</v>
-      </c>
-      <c r="K62">
-        <v>2.06</v>
-      </c>
-      <c r="L62" s="6">
-        <f t="shared" si="0"/>
-        <v>2.06</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="4">
-        <v>60</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C63" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="F63" s="1">
-        <v>7200</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="I63" s="15" t="s">
-        <v>339</v>
-      </c>
-      <c r="J63" s="1">
-        <v>4</v>
-      </c>
-      <c r="K63">
-        <v>0.68</v>
-      </c>
-      <c r="L63" s="6">
         <f t="shared" si="0"/>
         <v>2.72</v>
       </c>

</xml_diff>

<commit_message>
Updated 20 MHz crystal digi-key#.
</commit_message>
<xml_diff>
--- a/hardware/MainBoard/MainBoard_BOM.xlsx
+++ b/hardware/MainBoard/MainBoard_BOM.xlsx
@@ -100,9 +100,6 @@
     <t>Total Cost</t>
   </si>
   <si>
-    <t>Bill of Materials for 'Marote - Main Board (Rev A)'</t>
-  </si>
-  <si>
     <t>768-1101-1-ND</t>
   </si>
   <si>
@@ -1094,6 +1091,9 @@
   </si>
   <si>
     <t>CAP CER 0.33UF 16V 10% X5R 0402</t>
+  </si>
+  <si>
+    <t>Bill of Materials for 'Marmote - Main Board (Rev A)'</t>
   </si>
 </sst>
 </file>
@@ -1586,8 +1586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1609,7 +1609,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
-        <v>14</v>
+        <v>345</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -1666,28 +1666,28 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="E4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="G4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J4" s="1">
         <v>1</v>
@@ -1705,28 +1705,28 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="I5" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J5" s="1">
         <v>3</v>
@@ -1744,28 +1744,28 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" t="s">
         <v>340</v>
-      </c>
-      <c r="I6" t="s">
-        <v>341</v>
       </c>
       <c r="J6" s="1">
         <v>18</v>
@@ -1783,28 +1783,28 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="15" t="s">
         <v>220</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>221</v>
       </c>
       <c r="J7" s="1">
         <v>73</v>
@@ -1822,28 +1822,28 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="15" t="s">
         <v>225</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>226</v>
       </c>
       <c r="J8" s="1">
         <v>3</v>
@@ -1861,28 +1861,28 @@
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="15" t="s">
         <v>228</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>229</v>
       </c>
       <c r="J9" s="1">
         <v>4</v>
@@ -1900,28 +1900,28 @@
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="15" t="s">
         <v>231</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>232</v>
       </c>
       <c r="J10" s="1">
         <v>2</v>
@@ -1939,28 +1939,28 @@
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" t="s">
         <v>344</v>
-      </c>
-      <c r="I11" t="s">
-        <v>345</v>
       </c>
       <c r="J11" s="1">
         <v>7</v>
@@ -1978,20 +1978,20 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
       <c r="I12" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J12" s="12">
         <v>18</v>
@@ -2006,28 +2006,28 @@
         <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="15" t="s">
         <v>234</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>235</v>
       </c>
       <c r="J13" s="1">
         <v>8</v>
@@ -2045,28 +2045,28 @@
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="15" t="s">
         <v>237</v>
-      </c>
-      <c r="I14" s="15" t="s">
-        <v>238</v>
       </c>
       <c r="J14" s="1">
         <v>2</v>
@@ -2084,28 +2084,28 @@
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="15" t="s">
         <v>225</v>
-      </c>
-      <c r="I15" s="15" t="s">
-        <v>226</v>
       </c>
       <c r="J15" s="1">
         <v>2</v>
@@ -2123,28 +2123,28 @@
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="I16" s="15" t="s">
         <v>239</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="I16" s="15" t="s">
-        <v>240</v>
       </c>
       <c r="J16" s="1">
         <v>11</v>
@@ -2162,28 +2162,28 @@
         <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="I17" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J17" s="1">
         <v>1</v>
@@ -2201,28 +2201,28 @@
         <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="G18" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J18" s="1">
         <v>1</v>
@@ -2240,28 +2240,28 @@
         <v>16</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="G19" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J19" s="1">
         <v>1</v>
@@ -2279,28 +2279,28 @@
         <v>17</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="G20" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J20" s="1">
         <v>1</v>
@@ -2318,28 +2318,28 @@
         <v>18</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C21" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="I21" s="15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J21" s="1">
         <v>1</v>
@@ -2357,28 +2357,28 @@
         <v>19</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C22" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="E22" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>335</v>
-      </c>
       <c r="I22" s="15" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="J22" s="1">
         <v>2</v>
@@ -2393,28 +2393,28 @@
         <v>20</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="G23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H23" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="I23" s="15" t="s">
         <v>250</v>
-      </c>
-      <c r="I23" s="15" t="s">
-        <v>251</v>
       </c>
       <c r="J23" s="1">
         <v>1</v>
@@ -2432,28 +2432,28 @@
         <v>21</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="G24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H24" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="I24" s="15" t="s">
         <v>252</v>
-      </c>
-      <c r="I24" s="15" t="s">
-        <v>253</v>
       </c>
       <c r="J24" s="1">
         <v>1</v>
@@ -2471,28 +2471,28 @@
         <v>22</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H25" s="1" t="s">
+      <c r="I25" s="15" t="s">
         <v>255</v>
-      </c>
-      <c r="I25" s="15" t="s">
-        <v>256</v>
       </c>
       <c r="J25" s="1">
         <v>1</v>
@@ -2510,28 +2510,28 @@
         <v>23</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H26" s="1" t="s">
+      <c r="I26" s="15" t="s">
         <v>259</v>
-      </c>
-      <c r="I26" s="15" t="s">
-        <v>260</v>
       </c>
       <c r="J26" s="1">
         <v>6</v>
@@ -2549,28 +2549,28 @@
         <v>24</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C27" s="13">
         <v>24.9</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H27" s="1" t="s">
+      <c r="I27" s="15" t="s">
         <v>263</v>
-      </c>
-      <c r="I27" s="15" t="s">
-        <v>264</v>
       </c>
       <c r="J27" s="1">
         <v>8</v>
@@ -2588,28 +2588,28 @@
         <v>25</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F28" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H28" s="1" t="s">
+      <c r="I28" s="15" t="s">
         <v>266</v>
-      </c>
-      <c r="I28" s="15" t="s">
-        <v>267</v>
       </c>
       <c r="J28" s="1">
         <v>6</v>
@@ -2627,28 +2627,28 @@
         <v>26</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C29" s="13">
         <v>39</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F29" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="1" t="s">
+      <c r="I29" s="15" t="s">
         <v>269</v>
-      </c>
-      <c r="I29" s="15" t="s">
-        <v>270</v>
       </c>
       <c r="J29" s="1">
         <v>7</v>
@@ -2666,28 +2666,28 @@
         <v>27</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F30" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H30" s="1" t="s">
+      <c r="I30" s="15" t="s">
         <v>272</v>
-      </c>
-      <c r="I30" s="15" t="s">
-        <v>273</v>
       </c>
       <c r="J30" s="1">
         <v>1</v>
@@ -2705,28 +2705,28 @@
         <v>28</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F31" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="I31" s="15" t="s">
         <v>274</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="I31" s="15" t="s">
-        <v>275</v>
       </c>
       <c r="J31" s="1">
         <v>2</v>
@@ -2744,28 +2744,28 @@
         <v>29</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F32" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H32" s="1" t="s">
+      <c r="I32" s="15" t="s">
         <v>278</v>
-      </c>
-      <c r="I32" s="15" t="s">
-        <v>279</v>
       </c>
       <c r="J32" s="1">
         <v>4</v>
@@ -2783,28 +2783,28 @@
         <v>30</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C33" s="13">
         <v>22</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F33" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>282</v>
-      </c>
       <c r="I33" s="15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J33" s="1">
         <v>7</v>
@@ -2822,28 +2822,28 @@
         <v>31</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C34" s="13">
         <v>0</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F34" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H34" s="1" t="s">
+      <c r="I34" s="15" t="s">
         <v>284</v>
-      </c>
-      <c r="I34" s="15" t="s">
-        <v>285</v>
       </c>
       <c r="J34" s="1">
         <v>12</v>
@@ -2861,28 +2861,28 @@
         <v>32</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F35" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="G35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H35" s="1" t="s">
+      <c r="I35" s="15" t="s">
         <v>287</v>
-      </c>
-      <c r="I35" s="15" t="s">
-        <v>288</v>
       </c>
       <c r="J35" s="1">
         <v>7</v>
@@ -2900,28 +2900,28 @@
         <v>33</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F36" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H36" s="1" t="s">
+      <c r="I36" s="15" t="s">
         <v>290</v>
-      </c>
-      <c r="I36" s="15" t="s">
-        <v>291</v>
       </c>
       <c r="J36" s="1">
         <v>4</v>
@@ -2939,28 +2939,28 @@
         <v>34</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F37" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="G37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H37" s="1" t="s">
+      <c r="I37" s="15" t="s">
         <v>293</v>
-      </c>
-      <c r="I37" s="15" t="s">
-        <v>294</v>
       </c>
       <c r="J37" s="1">
         <v>1</v>
@@ -2978,28 +2978,28 @@
         <v>35</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F38" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H38" s="1" t="s">
+      <c r="I38" s="15" t="s">
         <v>296</v>
-      </c>
-      <c r="I38" s="15" t="s">
-        <v>297</v>
       </c>
       <c r="J38" s="1">
         <v>1</v>
@@ -3017,28 +3017,28 @@
         <v>36</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C39" s="13">
         <v>27</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F39" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H39" s="1" t="s">
+      <c r="I39" s="15" t="s">
         <v>299</v>
-      </c>
-      <c r="I39" s="15" t="s">
-        <v>300</v>
       </c>
       <c r="J39" s="1">
         <v>1</v>
@@ -3056,28 +3056,28 @@
         <v>37</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F40" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="G40" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H40" s="1" t="s">
+      <c r="I40" s="15" t="s">
         <v>302</v>
-      </c>
-      <c r="I40" s="15" t="s">
-        <v>303</v>
       </c>
       <c r="J40" s="1">
         <v>1</v>
@@ -3095,28 +3095,28 @@
         <v>38</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F41" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H41" s="1" t="s">
+      <c r="I41" s="15" t="s">
         <v>305</v>
-      </c>
-      <c r="I41" s="15" t="s">
-        <v>306</v>
       </c>
       <c r="J41" s="1">
         <v>1</v>
@@ -3134,28 +3134,28 @@
         <v>39</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C42" s="13">
         <v>100</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F42" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>308</v>
-      </c>
       <c r="I42" s="15" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J42" s="1">
         <v>3</v>
@@ -3173,28 +3173,28 @@
         <v>40</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C43" s="13">
         <v>330</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F43" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="G43" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H43" s="1" t="s">
+      <c r="I43" s="15" t="s">
         <v>310</v>
-      </c>
-      <c r="I43" s="15" t="s">
-        <v>311</v>
       </c>
       <c r="J43" s="1">
         <v>1</v>
@@ -3212,28 +3212,28 @@
         <v>41</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F44" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H44" s="1" t="s">
+      <c r="I44" s="15" t="s">
         <v>313</v>
-      </c>
-      <c r="I44" s="15" t="s">
-        <v>314</v>
       </c>
       <c r="J44" s="1">
         <v>2</v>
@@ -3251,20 +3251,20 @@
         <v>42</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
       <c r="H45" s="12"/>
       <c r="I45" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J45" s="12">
         <v>1</v>
@@ -3279,28 +3279,28 @@
         <v>43</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F46" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="G46" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H46" s="1" t="s">
+      <c r="I46" s="15" t="s">
         <v>316</v>
-      </c>
-      <c r="I46" s="15" t="s">
-        <v>317</v>
       </c>
       <c r="J46" s="1">
         <v>2</v>
@@ -3318,28 +3318,28 @@
         <v>44</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D47" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="F47" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>244</v>
-      </c>
       <c r="I47" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J47" s="1">
         <v>1</v>
@@ -3357,16 +3357,16 @@
         <v>45</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F48" s="1">
         <v>5009</v>
@@ -3375,10 +3375,10 @@
         <v>11</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I48" s="15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J48" s="1">
         <v>2</v>
@@ -3396,16 +3396,16 @@
         <v>46</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F49" s="1">
         <v>5121</v>
@@ -3414,10 +3414,10 @@
         <v>11</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I49" s="15" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J49" s="1">
         <v>2</v>
@@ -3438,25 +3438,25 @@
         <v>12</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I50" s="15" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J50" s="1">
         <v>1</v>
@@ -3474,28 +3474,28 @@
         <v>48</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I51" s="15" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J51" s="1">
         <v>2</v>
@@ -3513,28 +3513,28 @@
         <v>49</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I52" s="15" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J52" s="1">
         <v>1</v>
@@ -3552,28 +3552,28 @@
         <v>50</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E53" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I53" s="15" t="s">
         <v>16</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I53" s="15" t="s">
-        <v>17</v>
       </c>
       <c r="J53" s="1">
         <v>1</v>
@@ -3591,28 +3591,28 @@
         <v>51</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E54" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F54" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F54" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="G54" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I54" s="15" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="J54" s="1">
         <v>1</v>
@@ -3630,28 +3630,28 @@
         <v>52</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E55" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F55" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="G55" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I55" s="15" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J55" s="1">
         <v>1</v>
@@ -3669,28 +3669,28 @@
         <v>53</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E56" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F56" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="G56" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I56" s="15" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="J56" s="1">
         <v>1</v>
@@ -3708,28 +3708,28 @@
         <v>54</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I57" s="15" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J57" s="1">
         <v>1</v>
@@ -3747,28 +3747,28 @@
         <v>55</v>
       </c>
       <c r="B58" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H58" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C58" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="I58" s="15" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="J58" s="1">
         <v>1</v>
@@ -3786,28 +3786,28 @@
         <v>56</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E59" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F59" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="G59" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I59" s="15" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J59" s="1">
         <v>1</v>
@@ -3825,28 +3825,28 @@
         <v>57</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I60" s="15" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J60" s="1">
         <v>1</v>
@@ -3864,16 +3864,16 @@
         <v>58</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F61" s="1">
         <v>7200</v>
@@ -3882,10 +3882,10 @@
         <v>11</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I61" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="J61" s="1">
         <v>4</v>
@@ -3943,905 +3943,905 @@
         <v>8</v>
       </c>
       <c r="E1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>97</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>98</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>99</v>
-      </c>
-      <c r="J2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" t="s">
         <v>113</v>
-      </c>
-      <c r="C3" t="s">
-        <v>114</v>
       </c>
       <c r="D3">
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" t="s">
+        <v>98</v>
+      </c>
+      <c r="J3" t="s">
         <v>116</v>
-      </c>
-      <c r="H3" t="s">
-        <v>99</v>
-      </c>
-      <c r="J3" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4">
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5">
         <v>73</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6">
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8">
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="J10" t="s">
         <v>56</v>
-      </c>
-      <c r="J10" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11">
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12">
         <v>18</v>
       </c>
       <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" t="s">
         <v>26</v>
-      </c>
-      <c r="G12" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13">
         <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14">
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15">
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16">
         <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>198</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C17" t="s">
+        <v>197</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
         <v>199</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="C17" t="s">
-        <v>198</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>146</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C18" t="s">
+        <v>145</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
         <v>147</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="C18" t="s">
-        <v>146</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>148</v>
       </c>
-      <c r="F18" t="s">
+      <c r="H18" t="s">
         <v>149</v>
       </c>
-      <c r="H18" t="s">
+      <c r="J18" t="s">
         <v>150</v>
-      </c>
-      <c r="J18" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" t="s">
+        <v>139</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
         <v>141</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="C19" t="s">
-        <v>140</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>142</v>
       </c>
-      <c r="F19" t="s">
+      <c r="H19" t="s">
         <v>143</v>
       </c>
-      <c r="H19" t="s">
+      <c r="J19" t="s">
         <v>144</v>
-      </c>
-      <c r="J19" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" t="s">
+        <v>129</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
         <v>131</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C20" t="s">
-        <v>130</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>132</v>
       </c>
-      <c r="F20" t="s">
+      <c r="H20" t="s">
         <v>133</v>
       </c>
-      <c r="H20" t="s">
+      <c r="J20" t="s">
         <v>134</v>
-      </c>
-      <c r="J20" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>131</v>
+      </c>
+      <c r="F21" t="s">
         <v>137</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="C21" t="s">
-        <v>136</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>132</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="H21" t="s">
+        <v>133</v>
+      </c>
+      <c r="J21" t="s">
         <v>138</v>
-      </c>
-      <c r="H21" t="s">
-        <v>134</v>
-      </c>
-      <c r="J21" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>152</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C22" t="s">
+        <v>151</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
         <v>153</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="C22" t="s">
-        <v>152</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>154</v>
       </c>
-      <c r="F22" t="s">
+      <c r="H22" t="s">
         <v>155</v>
       </c>
-      <c r="H22" t="s">
-        <v>156</v>
-      </c>
       <c r="J22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B23" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" t="s">
         <v>85</v>
-      </c>
-      <c r="C23" t="s">
-        <v>86</v>
       </c>
       <c r="D23">
         <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J24" t="s">
         <v>34</v>
-      </c>
-      <c r="C24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>30</v>
-      </c>
-      <c r="H24" t="s">
-        <v>31</v>
-      </c>
-      <c r="J24" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
         <v>29</v>
       </c>
-      <c r="C25" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="H25" t="s">
         <v>30</v>
       </c>
-      <c r="H25" t="s">
+      <c r="J25" t="s">
         <v>31</v>
-      </c>
-      <c r="J25" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>193</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C26" t="s">
+        <v>192</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
         <v>194</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C26" t="s">
-        <v>193</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D27">
         <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B28" s="8">
         <v>24.9</v>
       </c>
       <c r="C28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D28">
         <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D29">
         <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B30" s="8">
         <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D30">
         <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B32" s="8">
         <v>110</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D32">
         <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B33" s="8">
         <v>49.9</v>
       </c>
       <c r="C33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D33">
         <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B34" s="8">
         <v>22</v>
       </c>
       <c r="C34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D34">
         <v>7</v>
       </c>
       <c r="E34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" s="8">
         <v>0</v>
       </c>
       <c r="C35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D35">
         <v>12</v>
       </c>
       <c r="E35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D36">
         <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D37">
         <v>4</v>
       </c>
       <c r="E37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B40" s="8">
         <v>27</v>
       </c>
       <c r="C40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B43" s="8">
         <v>100</v>
       </c>
       <c r="C43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D43">
         <v>3</v>
       </c>
       <c r="E43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B44" s="8">
         <v>330</v>
       </c>
       <c r="C44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C45" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D45">
         <v>2</v>
       </c>
       <c r="E45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B46" s="8">
         <v>0</v>
       </c>
       <c r="C46" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D46">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C47" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D47">
         <v>2</v>
       </c>
       <c r="E47" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C48" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D48">
         <v>2</v>
       </c>
       <c r="E48" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H48" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J48">
         <v>5009</v>
@@ -4849,25 +4849,25 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C49" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D49">
         <v>2</v>
       </c>
       <c r="E49" t="s">
+        <v>205</v>
+      </c>
+      <c r="F49" t="s">
         <v>206</v>
       </c>
-      <c r="F49" t="s">
+      <c r="H49" t="s">
         <v>207</v>
-      </c>
-      <c r="H49" t="s">
-        <v>208</v>
       </c>
       <c r="J49">
         <v>5121</v>
@@ -4878,305 +4878,305 @@
         <v>12</v>
       </c>
       <c r="B50" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C50" t="s">
+        <v>119</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50" t="s">
         <v>120</v>
       </c>
-      <c r="C50" t="s">
-        <v>120</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>121</v>
       </c>
-      <c r="F50" t="s">
+      <c r="H50" t="s">
         <v>122</v>
       </c>
-      <c r="H50" t="s">
-        <v>123</v>
-      </c>
       <c r="J50" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C51" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D51">
         <v>2</v>
       </c>
       <c r="E51" t="s">
+        <v>189</v>
+      </c>
+      <c r="F51" t="s">
         <v>190</v>
       </c>
-      <c r="F51" t="s">
+      <c r="H51" t="s">
+        <v>166</v>
+      </c>
+      <c r="J51" t="s">
         <v>191</v>
-      </c>
-      <c r="H51" t="s">
-        <v>167</v>
-      </c>
-      <c r="J51" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>212</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="C52" t="s">
+        <v>211</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52" t="s">
         <v>213</v>
       </c>
-      <c r="B52" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C52" t="s">
-        <v>212</v>
-      </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
         <v>214</v>
       </c>
-      <c r="F52" t="s">
+      <c r="H52" t="s">
         <v>215</v>
       </c>
-      <c r="H52" t="s">
-        <v>216</v>
-      </c>
       <c r="J52" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>184</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C53" t="s">
+        <v>183</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53" t="s">
         <v>185</v>
       </c>
-      <c r="B53" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="C53" t="s">
-        <v>184</v>
-      </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
+        <v>14</v>
+      </c>
+      <c r="H53" t="s">
+        <v>15</v>
+      </c>
+      <c r="I53" t="s">
         <v>186</v>
       </c>
-      <c r="F53" t="s">
-        <v>15</v>
-      </c>
-      <c r="H53" t="s">
-        <v>16</v>
-      </c>
-      <c r="I53" t="s">
-        <v>187</v>
-      </c>
       <c r="J53" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>157</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C54" t="s">
+        <v>156</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
         <v>158</v>
       </c>
-      <c r="B54" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="C54" t="s">
-        <v>157</v>
-      </c>
-      <c r="D54">
-        <v>1</v>
-      </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>159</v>
       </c>
-      <c r="F54" t="s">
+      <c r="H54" t="s">
         <v>160</v>
       </c>
-      <c r="H54" t="s">
+      <c r="J54" t="s">
         <v>161</v>
-      </c>
-      <c r="J54" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>101</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C55" t="s">
+        <v>100</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55" t="s">
         <v>102</v>
       </c>
-      <c r="B55" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C55" t="s">
-        <v>101</v>
-      </c>
-      <c r="D55">
-        <v>1</v>
-      </c>
-      <c r="E55" t="s">
+      <c r="F55" t="s">
         <v>103</v>
       </c>
-      <c r="F55" t="s">
+      <c r="H55" t="s">
         <v>104</v>
       </c>
-      <c r="H55" t="s">
+      <c r="J55" t="s">
         <v>105</v>
-      </c>
-      <c r="J55" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>163</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C56" t="s">
+        <v>162</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
         <v>164</v>
       </c>
-      <c r="B56" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="C56" t="s">
-        <v>163</v>
-      </c>
-      <c r="D56">
-        <v>1</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="F56" t="s">
         <v>165</v>
       </c>
-      <c r="F56" t="s">
+      <c r="H56" t="s">
         <v>166</v>
       </c>
-      <c r="H56" t="s">
+      <c r="J56" t="s">
         <v>167</v>
-      </c>
-      <c r="J56" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>179</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="C57" t="s">
+        <v>178</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57" t="s">
         <v>180</v>
       </c>
-      <c r="B57" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="C57" t="s">
-        <v>179</v>
-      </c>
-      <c r="D57">
-        <v>1</v>
-      </c>
-      <c r="E57" t="s">
+      <c r="F57" t="s">
         <v>181</v>
       </c>
-      <c r="F57" t="s">
+      <c r="H57" t="s">
+        <v>171</v>
+      </c>
+      <c r="J57" t="s">
         <v>182</v>
-      </c>
-      <c r="H57" t="s">
-        <v>172</v>
-      </c>
-      <c r="J57" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>169</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C58" t="s">
+        <v>168</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58" t="s">
+        <v>168</v>
+      </c>
+      <c r="F58" t="s">
         <v>170</v>
       </c>
-      <c r="B58" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="C58" t="s">
-        <v>169</v>
-      </c>
-      <c r="D58">
-        <v>1</v>
-      </c>
-      <c r="E58" t="s">
-        <v>169</v>
-      </c>
-      <c r="F58" t="s">
+      <c r="H58" t="s">
         <v>171</v>
       </c>
-      <c r="H58" t="s">
+      <c r="J58" t="s">
         <v>172</v>
-      </c>
-      <c r="J58" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>124</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C59" t="s">
+        <v>123</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59" t="s">
         <v>125</v>
       </c>
-      <c r="B59" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="C59" t="s">
-        <v>124</v>
-      </c>
-      <c r="D59">
-        <v>1</v>
-      </c>
-      <c r="E59" t="s">
+      <c r="F59" t="s">
         <v>126</v>
       </c>
-      <c r="F59" t="s">
+      <c r="H59" t="s">
         <v>127</v>
       </c>
-      <c r="H59" t="s">
+      <c r="J59" t="s">
         <v>128</v>
-      </c>
-      <c r="J59" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>174</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C60" t="s">
+        <v>173</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60" t="s">
         <v>175</v>
       </c>
-      <c r="B60" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="C60" t="s">
-        <v>174</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="E60" t="s">
+      <c r="F60" t="s">
         <v>176</v>
       </c>
-      <c r="F60" t="s">
+      <c r="H60" t="s">
+        <v>171</v>
+      </c>
+      <c r="J60" t="s">
         <v>177</v>
-      </c>
-      <c r="H60" t="s">
-        <v>172</v>
-      </c>
-      <c r="J60" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C61" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D61">
         <v>4</v>
       </c>
       <c r="E61" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected BOM file and schematic based on IES questions.
</commit_message>
<xml_diff>
--- a/hardware/MainBoard/MainBoard_BOM.xlsx
+++ b/hardware/MainBoard/MainBoard_BOM.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="348">
   <si>
     <t>Item #</t>
   </si>
@@ -1033,9 +1033,6 @@
     <t>IC ECONRST 3.3V W/PB 10% SOT23-3</t>
   </si>
   <si>
-    <t>CRYSTAL 16.000 MHZ 8PF SMD</t>
-  </si>
-  <si>
     <t>CRYSTAL 32.768 KHZ 7PF SMD</t>
   </si>
   <si>
@@ -1094,6 +1091,15 @@
   </si>
   <si>
     <t>Bill of Materials for 'Marmote - Main Board (Rev A)'</t>
+  </si>
+  <si>
+    <t>XC1556CT-ND</t>
+  </si>
+  <si>
+    <t>CRYSTAL 20.000 MHZ 8PF SMD</t>
+  </si>
+  <si>
+    <t>C29, C42, C46, C133, C135</t>
   </si>
 </sst>
 </file>
@@ -1229,7 +1235,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1271,6 +1277,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1584,10 +1591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,20 +1615,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
-        <v>345</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
+      <c r="A1" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -1735,7 +1742,7 @@
         <v>0.38</v>
       </c>
       <c r="L5" s="6">
-        <f t="shared" ref="L5:L61" si="0">J5*K5</f>
+        <f t="shared" ref="L5:L60" si="0">J5*K5</f>
         <v>1.1400000000000001</v>
       </c>
     </row>
@@ -1744,7 +1751,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>57</v>
@@ -1753,19 +1760,19 @@
         <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" t="s">
         <v>339</v>
-      </c>
-      <c r="I6" t="s">
-        <v>340</v>
       </c>
       <c r="J6" s="1">
         <v>18</v>
@@ -1822,7 +1829,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>42</v>
+        <v>347</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>41</v>
@@ -1846,14 +1853,14 @@
         <v>225</v>
       </c>
       <c r="J8" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K8">
         <v>0.08</v>
       </c>
       <c r="L8" s="6">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1935,7 +1942,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="5">
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1951,16 +1958,16 @@
         <v>217</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" t="s">
         <v>343</v>
-      </c>
-      <c r="I11" t="s">
-        <v>344</v>
       </c>
       <c r="J11" s="1">
         <v>7</v>
@@ -1996,13 +2003,13 @@
       <c r="J12" s="12">
         <v>18</v>
       </c>
-      <c r="L12" s="6">
+      <c r="L12" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="4">
         <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -2080,14 +2087,14 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="5">
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>72</v>
+        <v>335</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>23</v>
@@ -2096,26 +2103,26 @@
         <v>217</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>224</v>
+        <v>240</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>225</v>
+        <v>239</v>
       </c>
       <c r="J15" s="1">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="K15">
-        <v>0.08</v>
+        <v>0.53</v>
       </c>
       <c r="L15" s="6">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>5.83</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2123,116 +2130,116 @@
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>336</v>
+        <v>198</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>63</v>
+        <v>151</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>23</v>
+        <v>151</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>217</v>
+        <v>155</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="G16" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>240</v>
+        <v>154</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>239</v>
+        <v>153</v>
       </c>
       <c r="J16" s="1">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="K16">
-        <v>0.53</v>
+        <v>1.6</v>
       </c>
       <c r="L16" s="6">
-        <f t="shared" si="0"/>
-        <v>5.83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <f>J16*K16</f>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>198</v>
+        <v>146</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>153</v>
+        <v>245</v>
       </c>
       <c r="J17" s="1">
         <v>1</v>
       </c>
       <c r="K17">
-        <v>1.6</v>
+        <v>8.2100000000000009</v>
       </c>
       <c r="L17" s="6">
-        <f>J17*K17</f>
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>8.2100000000000009</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="J18" s="1">
         <v>1</v>
       </c>
       <c r="K18">
-        <v>8.2100000000000009</v>
+        <v>3.45</v>
       </c>
       <c r="L18" s="6">
         <f t="shared" si="0"/>
-        <v>8.2100000000000009</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -2240,38 +2247,38 @@
         <v>16</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J19" s="1">
         <v>1</v>
       </c>
       <c r="K19">
-        <v>3.45</v>
+        <v>5.81</v>
       </c>
       <c r="L19" s="6">
         <f t="shared" si="0"/>
-        <v>3.45</v>
+        <v>5.81</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2279,38 +2286,38 @@
         <v>17</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>133</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="J20" s="1">
         <v>1</v>
       </c>
       <c r="K20">
-        <v>5.81</v>
+        <v>6.24</v>
       </c>
       <c r="L20" s="6">
         <f t="shared" si="0"/>
-        <v>5.81</v>
+        <v>6.24</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2318,38 +2325,35 @@
         <v>18</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>135</v>
+        <v>84</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>133</v>
+        <v>332</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G21" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>137</v>
+        <v>333</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>248</v>
+        <v>330</v>
       </c>
       <c r="J21" s="1">
-        <v>1</v>
-      </c>
-      <c r="K21">
-        <v>6.24</v>
+        <v>2</v>
       </c>
       <c r="L21" s="6">
         <f t="shared" si="0"/>
-        <v>6.24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2357,74 +2361,77 @@
         <v>19</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>84</v>
+        <v>33</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>333</v>
+        <v>30</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>332</v>
+        <v>34</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>334</v>
+        <v>249</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>331</v>
+        <v>250</v>
       </c>
       <c r="J22" s="1">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>0.6</v>
       </c>
       <c r="L22" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="A23" s="5">
         <v>20</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="J23" s="1">
         <v>1</v>
       </c>
       <c r="K23">
-        <v>0.6</v>
+        <v>0.33</v>
       </c>
       <c r="L23" s="6">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -2432,155 +2439,155 @@
         <v>21</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>27</v>
+        <v>193</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>192</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>27</v>
+        <v>192</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>30</v>
+        <v>253</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>31</v>
+        <v>192</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="J24" s="1">
         <v>1</v>
       </c>
       <c r="K24">
-        <v>0.33</v>
+        <v>0.37</v>
       </c>
       <c r="L24" s="6">
         <f t="shared" si="0"/>
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
         <v>22</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>193</v>
+        <v>70</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>192</v>
+        <v>69</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>192</v>
+        <v>35</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>192</v>
+        <v>256</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="I25" s="15" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="J25" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K25">
-        <v>0.37</v>
+        <v>2.3E-2</v>
       </c>
       <c r="L25" s="6">
         <f t="shared" si="0"/>
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0.13800000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>23</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>69</v>
+        <v>82</v>
+      </c>
+      <c r="C26" s="13">
+        <v>24.9</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="I26" s="15" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="J26" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K26">
-        <v>2.3E-2</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="L26" s="6">
         <f t="shared" si="0"/>
-        <v>0.13800000000000001</v>
+        <v>0.66400000000000003</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="A27" s="5">
         <v>24</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="13">
-        <v>24.9</v>
+        <v>109</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>108</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="I27" s="15" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="J27" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K27">
-        <v>8.3000000000000004E-2</v>
+        <v>0.123</v>
       </c>
       <c r="L27" s="6">
         <f t="shared" si="0"/>
-        <v>0.66400000000000003</v>
+        <v>0.73799999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -2588,10 +2595,10 @@
         <v>25</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>108</v>
+        <v>88</v>
+      </c>
+      <c r="C28" s="13">
+        <v>39</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>35</v>
@@ -2600,26 +2607,26 @@
         <v>257</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="J28" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K28">
-        <v>0.123</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="L28" s="6">
         <f t="shared" si="0"/>
-        <v>0.73799999999999999</v>
+        <v>0.182</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -2627,10 +2634,10 @@
         <v>26</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C29" s="13">
-        <v>39</v>
+        <v>48</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>35</v>
@@ -2639,26 +2646,26 @@
         <v>257</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="I29" s="15" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="J29" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="K29">
-        <v>2.5999999999999999E-2</v>
+        <v>0.123</v>
       </c>
       <c r="L29" s="6">
         <f t="shared" si="0"/>
-        <v>0.182</v>
+        <v>0.123</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2666,10 +2673,10 @@
         <v>27</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>35</v>
@@ -2678,26 +2685,26 @@
         <v>257</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="J30" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K30">
-        <v>0.123</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="L30" s="6">
         <f t="shared" si="0"/>
-        <v>0.123</v>
+        <v>0.40200000000000002</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2705,10 +2712,10 @@
         <v>28</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>35</v>
@@ -2717,26 +2724,26 @@
         <v>257</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="I31" s="15" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="J31" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K31">
-        <v>0.20100000000000001</v>
+        <v>2.3E-2</v>
       </c>
       <c r="L31" s="6">
         <f t="shared" si="0"/>
-        <v>0.40200000000000002</v>
+        <v>9.1999999999999998E-2</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2744,10 +2751,10 @@
         <v>29</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>91</v>
+        <v>79</v>
+      </c>
+      <c r="C32" s="13">
+        <v>22</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>35</v>
@@ -2756,26 +2763,26 @@
         <v>257</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="J32" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K32">
         <v>2.3E-2</v>
       </c>
       <c r="L32" s="6">
         <f t="shared" si="0"/>
-        <v>9.1999999999999998E-2</v>
+        <v>0.161</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2783,10 +2790,10 @@
         <v>30</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>79</v>
+        <v>36</v>
       </c>
       <c r="C33" s="13">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>35</v>
@@ -2795,26 +2802,26 @@
         <v>257</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="I33" s="15" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="J33" s="1">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="K33">
-        <v>2.3E-2</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="L33" s="6">
         <f t="shared" si="0"/>
-        <v>0.161</v>
+        <v>2.1719999999999997</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2822,10 +2829,10 @@
         <v>31</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="13">
-        <v>0</v>
+        <v>52</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>35</v>
@@ -2834,37 +2841,37 @@
         <v>257</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="J34" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="K34">
-        <v>0.18099999999999999</v>
+        <v>2.3E-2</v>
       </c>
       <c r="L34" s="6">
         <f t="shared" si="0"/>
-        <v>2.1719999999999997</v>
+        <v>0.161</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+      <c r="A35" s="5">
         <v>32</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>35</v>
@@ -2873,26 +2880,26 @@
         <v>257</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="I35" s="15" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="J35" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K35">
-        <v>2.3E-2</v>
+        <v>0.123</v>
       </c>
       <c r="L35" s="6">
         <f t="shared" si="0"/>
-        <v>0.161</v>
+        <v>0.49199999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2900,49 +2907,49 @@
         <v>33</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="I36" s="15" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="J36" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K36">
-        <v>0.123</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="L36" s="6">
         <f t="shared" si="0"/>
-        <v>0.49199999999999999</v>
+        <v>8.3000000000000004E-2</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
+      <c r="A37" s="4">
         <v>34</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>35</v>
@@ -2951,16 +2958,16 @@
         <v>260</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="J37" s="1">
         <v>1</v>
@@ -2978,10 +2985,10 @@
         <v>35</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+      <c r="C38" s="13">
+        <v>27</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>35</v>
@@ -2990,16 +2997,16 @@
         <v>260</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="J38" s="1">
         <v>1</v>
@@ -3013,14 +3020,14 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
+      <c r="A39" s="5">
         <v>36</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C39" s="13">
-        <v>27</v>
+        <v>90</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>89</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>35</v>
@@ -3029,16 +3036,16 @@
         <v>260</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="I39" s="15" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="J39" s="1">
         <v>1</v>
@@ -3056,10 +3063,10 @@
         <v>37</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>35</v>
@@ -3068,16 +3075,16 @@
         <v>260</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="I40" s="15" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="J40" s="1">
         <v>1</v>
@@ -3095,10 +3102,10 @@
         <v>38</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>59</v>
+        <v>107</v>
+      </c>
+      <c r="C41" s="13">
+        <v>100</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>35</v>
@@ -3107,26 +3114,26 @@
         <v>260</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="I41" s="15" t="s">
-        <v>305</v>
+        <v>274</v>
       </c>
       <c r="J41" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K41">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="L41" s="6">
         <f t="shared" si="0"/>
-        <v>8.3000000000000004E-2</v>
+        <v>0.249</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -3134,10 +3141,10 @@
         <v>39</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C42" s="13">
-        <v>100</v>
+        <v>330</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>35</v>
@@ -3146,26 +3153,26 @@
         <v>260</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="I42" s="15" t="s">
-        <v>274</v>
+        <v>310</v>
       </c>
       <c r="J42" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K42">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="L42" s="6">
         <f t="shared" si="0"/>
-        <v>0.249</v>
+        <v>8.3000000000000004E-2</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -3173,10 +3180,10 @@
         <v>40</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C43" s="13">
-        <v>330</v>
+        <v>62</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>35</v>
@@ -3185,93 +3192,93 @@
         <v>260</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="I43" s="15" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="J43" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K43">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="L43" s="6">
         <f t="shared" si="0"/>
-        <v>8.3000000000000004E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
+        <v>0.16600000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="11">
         <v>41</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="I44" s="15" t="s">
-        <v>313</v>
-      </c>
-      <c r="J44" s="1">
+      <c r="B44" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="J44" s="12">
+        <v>1</v>
+      </c>
+      <c r="L44" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
+        <v>42</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="I45" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="J45" s="1">
         <v>2</v>
       </c>
-      <c r="K44">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="L44" s="6">
-        <f t="shared" si="0"/>
-        <v>0.16600000000000001</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="11">
-        <v>42</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E45" s="1"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="J45" s="12">
-        <v>1</v>
+      <c r="K45">
+        <v>0.29099999999999998</v>
       </c>
       <c r="L45" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.58199999999999996</v>
       </c>
     </row>
     <row r="46" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3279,77 +3286,77 @@
         <v>43</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>201</v>
+        <v>334</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>200</v>
+        <v>241</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>317</v>
+        <v>242</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>314</v>
+        <v>244</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>315</v>
+        <v>243</v>
       </c>
       <c r="I46" s="15" t="s">
-        <v>316</v>
+        <v>199</v>
       </c>
       <c r="J46" s="1">
+        <v>1</v>
+      </c>
+      <c r="K46">
+        <v>0.97</v>
+      </c>
+      <c r="L46" s="6">
+        <f>J46*K46</f>
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
+        <v>44</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F47" s="1">
+        <v>5009</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="I47" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="J47" s="1">
         <v>2</v>
       </c>
-      <c r="K46">
-        <v>0.29099999999999998</v>
-      </c>
-      <c r="L46" s="6">
-        <f t="shared" si="0"/>
-        <v>0.58199999999999996</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
-        <v>44</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="I47" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="J47" s="1">
-        <v>1</v>
-      </c>
       <c r="K47">
-        <v>0.97</v>
+        <v>0.35</v>
       </c>
       <c r="L47" s="6">
-        <f>J47*K47</f>
-        <v>0.97</v>
+        <f t="shared" si="0"/>
+        <v>0.7</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -3357,28 +3364,28 @@
         <v>45</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>207</v>
       </c>
       <c r="F48" s="1">
-        <v>5009</v>
+        <v>5121</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="I48" s="15" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="J48" s="1">
         <v>2</v>
@@ -3392,42 +3399,42 @@
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="5">
+      <c r="A49" s="4">
         <v>46</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>204</v>
+        <v>12</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>203</v>
+        <v>119</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>203</v>
+        <v>119</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="F49" s="1">
-        <v>5121</v>
+        <v>122</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>119</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>206</v>
+        <v>121</v>
       </c>
       <c r="I49" s="15" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="J49" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K49">
-        <v>0.35</v>
+        <v>53.91</v>
       </c>
       <c r="L49" s="6">
         <f t="shared" si="0"/>
-        <v>0.7</v>
+        <v>53.91</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -3435,77 +3442,77 @@
         <v>47</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>12</v>
+        <v>188</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>119</v>
+        <v>187</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>119</v>
+        <v>187</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>122</v>
+        <v>166</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>119</v>
+        <v>191</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>121</v>
+        <v>190</v>
       </c>
       <c r="I50" s="15" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="J50" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K50">
-        <v>53.91</v>
+        <v>20.09</v>
       </c>
       <c r="L50" s="6">
         <f t="shared" si="0"/>
-        <v>53.91</v>
+        <v>40.18</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
+      <c r="A51" s="5">
         <v>48</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>166</v>
+        <v>215</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="I51" s="15" t="s">
-        <v>321</v>
+        <v>211</v>
       </c>
       <c r="J51" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K51">
-        <v>20.09</v>
+        <v>0.95</v>
       </c>
       <c r="L51" s="6">
         <f t="shared" si="0"/>
-        <v>40.18</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -3513,38 +3520,38 @@
         <v>49</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>212</v>
+        <v>184</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>211</v>
+        <v>183</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>211</v>
+        <v>183</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>215</v>
+        <v>15</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>211</v>
+        <v>14</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>214</v>
+        <v>14</v>
       </c>
       <c r="I52" s="15" t="s">
-        <v>211</v>
+        <v>16</v>
       </c>
       <c r="J52" s="1">
         <v>1</v>
       </c>
       <c r="K52">
-        <v>0.95</v>
+        <v>4.25</v>
       </c>
       <c r="L52" s="6">
         <f t="shared" si="0"/>
-        <v>0.95</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -3552,38 +3559,38 @@
         <v>50</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>183</v>
+        <v>156</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>183</v>
+        <v>156</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>15</v>
+        <v>160</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>14</v>
+        <v>161</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>14</v>
+        <v>159</v>
       </c>
       <c r="I53" s="15" t="s">
-        <v>16</v>
+        <v>322</v>
       </c>
       <c r="J53" s="1">
         <v>1</v>
       </c>
       <c r="K53">
-        <v>4.25</v>
+        <v>6.66</v>
       </c>
       <c r="L53" s="6">
         <f t="shared" si="0"/>
-        <v>4.25</v>
+        <v>6.66</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -3591,142 +3598,142 @@
         <v>51</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>157</v>
+        <v>101</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>156</v>
+        <v>100</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>156</v>
+        <v>100</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>160</v>
+        <v>104</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>161</v>
+        <v>105</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>159</v>
+        <v>103</v>
       </c>
       <c r="I54" s="15" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="J54" s="1">
         <v>1</v>
       </c>
       <c r="K54">
-        <v>6.66</v>
+        <v>0.34</v>
       </c>
       <c r="L54" s="6">
         <f t="shared" si="0"/>
-        <v>6.66</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>52</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>101</v>
+        <v>163</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>100</v>
+        <v>162</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>100</v>
+        <v>162</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>104</v>
+        <v>166</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>105</v>
+        <v>167</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>103</v>
+        <v>165</v>
       </c>
       <c r="I55" s="15" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="J55" s="1">
         <v>1</v>
       </c>
       <c r="K55">
-        <v>0.34</v>
+        <v>0.81</v>
       </c>
       <c r="L55" s="6">
         <f t="shared" si="0"/>
-        <v>0.34</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>53</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>165</v>
+        <v>345</v>
       </c>
       <c r="I56" s="15" t="s">
-        <v>324</v>
+        <v>346</v>
       </c>
       <c r="J56" s="1">
         <v>1</v>
       </c>
       <c r="K56">
-        <v>0.81</v>
+        <v>4.3099999999999996</v>
       </c>
       <c r="L56" s="6">
         <f t="shared" si="0"/>
-        <v>0.81</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+        <v>4.3099999999999996</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>54</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>171</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="I57" s="15" t="s">
         <v>325</v>
@@ -3735,11 +3742,11 @@
         <v>1</v>
       </c>
       <c r="K57">
-        <v>4.3099999999999996</v>
+        <v>1.58</v>
       </c>
       <c r="L57" s="6">
         <f t="shared" si="0"/>
-        <v>4.3099999999999996</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="58" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3747,25 +3754,25 @@
         <v>55</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>169</v>
+        <v>124</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>168</v>
+        <v>123</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>168</v>
+        <v>123</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>172</v>
+        <v>128</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="I58" s="15" t="s">
         <v>326</v>
@@ -3774,37 +3781,37 @@
         <v>1</v>
       </c>
       <c r="K58">
-        <v>1.58</v>
+        <v>2.59</v>
       </c>
       <c r="L58" s="6">
         <f t="shared" si="0"/>
-        <v>1.58</v>
+        <v>2.59</v>
       </c>
     </row>
     <row r="59" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="4">
+      <c r="A59" s="5">
         <v>56</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>124</v>
+        <v>174</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>123</v>
+        <v>173</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>123</v>
+        <v>173</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>127</v>
+        <v>171</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>128</v>
+        <v>177</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>126</v>
+        <v>176</v>
       </c>
       <c r="I59" s="15" t="s">
         <v>327</v>
@@ -3813,87 +3820,48 @@
         <v>1</v>
       </c>
       <c r="K59">
-        <v>2.59</v>
+        <v>2.06</v>
       </c>
       <c r="L59" s="6">
         <f t="shared" si="0"/>
-        <v>2.59</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>2.06</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>57</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>174</v>
+        <v>216</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>173</v>
+        <v>19</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>173</v>
+        <v>195</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="G60" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F60" s="1">
+        <v>7200</v>
+      </c>
+      <c r="G60" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>176</v>
+        <v>329</v>
       </c>
       <c r="I60" s="15" t="s">
         <v>328</v>
       </c>
       <c r="J60" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K60">
-        <v>2.06</v>
+        <v>0.68</v>
       </c>
       <c r="L60" s="6">
-        <f t="shared" si="0"/>
-        <v>2.06</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" s="5">
-        <v>58</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="C61" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="F61" s="1">
-        <v>7200</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="I61" s="15" t="s">
-        <v>329</v>
-      </c>
-      <c r="J61" s="1">
-        <v>4</v>
-      </c>
-      <c r="K61">
-        <v>0.68</v>
-      </c>
-      <c r="L61" s="6">
         <f t="shared" si="0"/>
         <v>2.72</v>
       </c>

</xml_diff>

<commit_message>
Corrected ETH PHY R_BIAS value in MainBoard main branch BOM file.
</commit_message>
<xml_diff>
--- a/hardware/MainBoard/MainBoard_BOM.xlsx
+++ b/hardware/MainBoard/MainBoard_BOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="19440" windowHeight="12240" tabRatio="491"/>
@@ -931,15 +931,6 @@
     <t>RES 1.00K OHM 1/16W 1% 0402 SMD</t>
   </si>
   <si>
-    <t>CRCW04024R87FKED</t>
-  </si>
-  <si>
-    <t>541-4.87LLCT-ND</t>
-  </si>
-  <si>
-    <t>RES 4.87 OHM 1/16W 1% 0402 SMD</t>
-  </si>
-  <si>
     <t>CRCW040212K0FKED</t>
   </si>
   <si>
@@ -1090,9 +1081,6 @@
     <t>CAP CER 0.33UF 16V 10% X5R 0402</t>
   </si>
   <si>
-    <t>Bill of Materials for 'Marmote - Main Board (Rev A)'</t>
-  </si>
-  <si>
     <t>XC1556CT-ND</t>
   </si>
   <si>
@@ -1100,6 +1088,18 @@
   </si>
   <si>
     <t>C29, C42, C46, C133, C135</t>
+  </si>
+  <si>
+    <t>RES 4.87K OHM 1/16W 1% 0402 SMD</t>
+  </si>
+  <si>
+    <t>CRCW04024K87FKED</t>
+  </si>
+  <si>
+    <t>541-4.87KLCT-ND</t>
+  </si>
+  <si>
+    <t>Bill of Materials for 'Marmote - Main Board (Teton)'</t>
   </si>
 </sst>
 </file>
@@ -1594,7 +1594,7 @@
   <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1616,7 +1616,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -1751,7 +1751,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>57</v>
@@ -1760,19 +1760,19 @@
         <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="I6" t="s">
         <v>336</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="I6" t="s">
-        <v>339</v>
       </c>
       <c r="J6" s="1">
         <v>18</v>
@@ -1829,7 +1829,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>41</v>
@@ -1958,16 +1958,16 @@
         <v>217</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="I11" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="J11" s="1">
         <v>7</v>
@@ -2091,7 +2091,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>63</v>
@@ -2334,19 +2334,19 @@
         <v>85</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="J21" s="1">
         <v>2</v>
@@ -2919,16 +2919,16 @@
         <v>260</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>291</v>
+        <v>345</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>292</v>
+        <v>346</v>
       </c>
       <c r="I36" s="15" t="s">
-        <v>293</v>
+        <v>344</v>
       </c>
       <c r="J36" s="1">
         <v>1</v>
@@ -2958,16 +2958,16 @@
         <v>260</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="J37" s="1">
         <v>1</v>
@@ -2997,16 +2997,16 @@
         <v>260</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="J38" s="1">
         <v>1</v>
@@ -3036,16 +3036,16 @@
         <v>260</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="I39" s="15" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="J39" s="1">
         <v>1</v>
@@ -3075,16 +3075,16 @@
         <v>260</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="I40" s="15" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="J40" s="1">
         <v>1</v>
@@ -3114,13 +3114,13 @@
         <v>260</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="I41" s="15" t="s">
         <v>274</v>
@@ -3153,16 +3153,16 @@
         <v>260</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="I42" s="15" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="J42" s="1">
         <v>1</v>
@@ -3192,16 +3192,16 @@
         <v>260</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="I43" s="15" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="J43" s="1">
         <v>2</v>
@@ -3256,19 +3256,19 @@
         <v>200</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I45" s="15" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="J45" s="1">
         <v>2</v>
@@ -3286,7 +3286,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C46" s="13" t="s">
         <v>197</v>
@@ -3346,7 +3346,7 @@
         <v>210</v>
       </c>
       <c r="I47" s="15" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="J47" s="1">
         <v>2</v>
@@ -3385,7 +3385,7 @@
         <v>206</v>
       </c>
       <c r="I48" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J48" s="1">
         <v>2</v>
@@ -3424,7 +3424,7 @@
         <v>121</v>
       </c>
       <c r="I49" s="15" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="J49" s="1">
         <v>1</v>
@@ -3463,7 +3463,7 @@
         <v>190</v>
       </c>
       <c r="I50" s="15" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="J50" s="1">
         <v>2</v>
@@ -3580,7 +3580,7 @@
         <v>159</v>
       </c>
       <c r="I53" s="15" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="J53" s="1">
         <v>1</v>
@@ -3619,7 +3619,7 @@
         <v>103</v>
       </c>
       <c r="I54" s="15" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="J54" s="1">
         <v>1</v>
@@ -3658,7 +3658,7 @@
         <v>165</v>
       </c>
       <c r="I55" s="15" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="J55" s="1">
         <v>1</v>
@@ -3694,10 +3694,10 @@
         <v>11</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="I56" s="15" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="J56" s="1">
         <v>1</v>
@@ -3736,7 +3736,7 @@
         <v>170</v>
       </c>
       <c r="I57" s="15" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="J57" s="1">
         <v>1</v>
@@ -3775,7 +3775,7 @@
         <v>126</v>
       </c>
       <c r="I58" s="15" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="J58" s="1">
         <v>1</v>
@@ -3814,7 +3814,7 @@
         <v>176</v>
       </c>
       <c r="I59" s="15" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="J59" s="1">
         <v>1</v>
@@ -3850,10 +3850,10 @@
         <v>11</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="I60" s="15" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="J60" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
Modified R14 to DNP in the BOM file.
</commit_message>
<xml_diff>
--- a/hardware/MainBoard/MainBoard_BOM.xlsx
+++ b/hardware/MainBoard/MainBoard_BOM.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="350">
   <si>
     <t>Item #</t>
   </si>
@@ -1100,6 +1100,12 @@
   </si>
   <si>
     <t>Bill of Materials for 'Marmote - Main Board (Teton)'</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>R4, R11, R12, R13, R15, R16, R17, R18, R49, R74, R75</t>
   </si>
 </sst>
 </file>
@@ -1591,10 +1597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L60"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1742,7 +1748,7 @@
         <v>0.38</v>
       </c>
       <c r="L5" s="6">
-        <f t="shared" ref="L5:L60" si="0">J5*K5</f>
+        <f t="shared" ref="L5:L61" si="0">J5*K5</f>
         <v>1.1400000000000001</v>
       </c>
     </row>
@@ -2790,7 +2796,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>36</v>
+        <v>349</v>
       </c>
       <c r="C33" s="13">
         <v>0</v>
@@ -2820,58 +2826,58 @@
         <v>0.18099999999999999</v>
       </c>
       <c r="L33" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="L33" si="1">J33*K33</f>
         <v>2.1719999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+    <row r="34" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11">
+        <v>30</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="I34" s="16" t="s">
+        <v>284</v>
+      </c>
+      <c r="J34" s="12">
+        <v>1</v>
+      </c>
+      <c r="K34" s="2">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="L34" s="17">
+        <f t="shared" si="0"/>
+        <v>0.18099999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
         <v>31</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C35" s="13" t="s">
         <v>51</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="I34" s="15" t="s">
-        <v>287</v>
-      </c>
-      <c r="J34" s="1">
-        <v>7</v>
-      </c>
-      <c r="K34">
-        <v>2.3E-2</v>
-      </c>
-      <c r="L34" s="6">
-        <f t="shared" si="0"/>
-        <v>0.161</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
-        <v>32</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>49</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>35</v>
@@ -2880,76 +2886,76 @@
         <v>257</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="I35" s="15" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="J35" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K35">
-        <v>0.123</v>
+        <v>2.3E-2</v>
       </c>
       <c r="L35" s="6">
         <f t="shared" si="0"/>
-        <v>0.49199999999999999</v>
+        <v>0.161</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
-        <v>33</v>
+      <c r="A36" s="5">
+        <v>32</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>345</v>
+        <v>288</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>346</v>
+        <v>289</v>
       </c>
       <c r="I36" s="15" t="s">
-        <v>344</v>
+        <v>290</v>
       </c>
       <c r="J36" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K36">
-        <v>8.3000000000000004E-2</v>
+        <v>0.123</v>
       </c>
       <c r="L36" s="6">
         <f t="shared" si="0"/>
-        <v>8.3000000000000004E-2</v>
+        <v>0.49199999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>35</v>
@@ -2958,16 +2964,16 @@
         <v>260</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>291</v>
+        <v>345</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>292</v>
+        <v>346</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>293</v>
+        <v>344</v>
       </c>
       <c r="J37" s="1">
         <v>1</v>
@@ -2982,13 +2988,13 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C38" s="13">
-        <v>27</v>
+        <v>78</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>77</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>35</v>
@@ -2997,16 +3003,16 @@
         <v>260</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="J38" s="1">
         <v>1</v>
@@ -3020,14 +3026,14 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
-        <v>36</v>
+      <c r="A39" s="4">
+        <v>35</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>89</v>
+        <v>83</v>
+      </c>
+      <c r="C39" s="13">
+        <v>27</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>35</v>
@@ -3036,16 +3042,16 @@
         <v>260</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="I39" s="15" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="J39" s="1">
         <v>1</v>
@@ -3059,14 +3065,14 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
-        <v>37</v>
+      <c r="A40" s="5">
+        <v>36</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>35</v>
@@ -3075,16 +3081,16 @@
         <v>260</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="I40" s="15" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="J40" s="1">
         <v>1</v>
@@ -3098,14 +3104,14 @@
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
-        <v>38</v>
+      <c r="A41" s="4">
+        <v>37</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C41" s="13">
-        <v>100</v>
+        <v>60</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>35</v>
@@ -3114,37 +3120,37 @@
         <v>260</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="I41" s="15" t="s">
-        <v>274</v>
+        <v>302</v>
       </c>
       <c r="J41" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K41">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="L41" s="6">
         <f t="shared" si="0"/>
-        <v>0.249</v>
+        <v>8.3000000000000004E-2</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
-        <v>39</v>
+      <c r="A42" s="5">
+        <v>38</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C42" s="13">
-        <v>330</v>
+        <v>100</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>35</v>
@@ -3153,37 +3159,37 @@
         <v>260</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I42" s="15" t="s">
-        <v>307</v>
+        <v>274</v>
       </c>
       <c r="J42" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K42">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="L42" s="6">
         <f t="shared" si="0"/>
-        <v>8.3000000000000004E-2</v>
+        <v>0.249</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>61</v>
+        <v>111</v>
+      </c>
+      <c r="C43" s="13">
+        <v>330</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>35</v>
@@ -3192,200 +3198,200 @@
         <v>260</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="I43" s="15" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="J43" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K43">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="L43" s="6">
         <f t="shared" si="0"/>
+        <v>8.3000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>40</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="I44" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="J44" s="1">
+        <v>2</v>
+      </c>
+      <c r="K44">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="L44" s="6">
+        <f t="shared" si="0"/>
         <v>0.16600000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="11">
+    <row r="45" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="11">
         <v>41</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C45" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="D45" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="16" t="s">
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="J44" s="12">
-        <v>1</v>
-      </c>
-      <c r="L44" s="17">
+      <c r="J45" s="12">
+        <v>1</v>
+      </c>
+      <c r="L45" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="5">
+    <row r="46" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
         <v>42</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="C46" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H45" s="1" t="s">
+      <c r="G46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="I45" s="15" t="s">
+      <c r="I46" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="J45" s="1">
+      <c r="J46" s="1">
         <v>2</v>
       </c>
-      <c r="K45">
+      <c r="K46">
         <v>0.29099999999999998</v>
       </c>
-      <c r="L45" s="6">
+      <c r="L46" s="6">
         <f t="shared" si="0"/>
         <v>0.58199999999999996</v>
       </c>
     </row>
-    <row r="46" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
+    <row r="47" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
         <v>43</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C47" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="G46" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H46" s="1" t="s">
+      <c r="G47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="I46" s="15" t="s">
+      <c r="I47" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="J46" s="1">
-        <v>1</v>
-      </c>
-      <c r="K46">
+      <c r="J47" s="1">
+        <v>1</v>
+      </c>
+      <c r="K47">
         <v>0.97</v>
       </c>
-      <c r="L46" s="6">
-        <f>J46*K46</f>
+      <c r="L47" s="6">
+        <f>J47*K47</f>
         <v>0.97</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="5">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="5">
         <v>44</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B48" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C48" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="F47" s="1">
-        <v>5009</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="I47" s="15" t="s">
-        <v>315</v>
-      </c>
-      <c r="J47" s="1">
-        <v>2</v>
-      </c>
-      <c r="K47">
-        <v>0.35</v>
-      </c>
-      <c r="L47" s="6">
-        <f t="shared" si="0"/>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
-        <v>45</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>207</v>
       </c>
       <c r="F48" s="1">
-        <v>5121</v>
+        <v>5009</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="I48" s="15" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J48" s="1">
         <v>2</v>
@@ -3400,468 +3406,507 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>12</v>
+        <v>204</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>119</v>
+        <v>203</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>119</v>
+        <v>203</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>119</v>
+        <v>207</v>
+      </c>
+      <c r="F49" s="1">
+        <v>5121</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>121</v>
+        <v>206</v>
       </c>
       <c r="I49" s="15" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="J49" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K49">
-        <v>53.91</v>
+        <v>0.35</v>
       </c>
       <c r="L49" s="6">
         <f t="shared" si="0"/>
-        <v>53.91</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
+        <v>46</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I50" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="J50" s="1">
+        <v>1</v>
+      </c>
+      <c r="K50">
+        <v>53.91</v>
+      </c>
+      <c r="L50" s="6">
+        <f t="shared" si="0"/>
+        <v>53.91</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
         <v>47</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B51" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C51" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="G50" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H50" s="1" t="s">
+      <c r="G51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H51" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="I50" s="15" t="s">
+      <c r="I51" s="15" t="s">
         <v>318</v>
       </c>
-      <c r="J50" s="1">
+      <c r="J51" s="1">
         <v>2</v>
       </c>
-      <c r="K50">
+      <c r="K51">
         <v>20.09</v>
       </c>
-      <c r="L50" s="6">
+      <c r="L51" s="6">
         <f t="shared" si="0"/>
         <v>40.18</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="5">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="5">
         <v>48</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B52" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C52" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F52" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="G51" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H51" s="1" t="s">
+      <c r="G52" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H52" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="I51" s="15" t="s">
+      <c r="I52" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="J51" s="1">
-        <v>1</v>
-      </c>
-      <c r="K51">
+      <c r="J52" s="1">
+        <v>1</v>
+      </c>
+      <c r="K52">
         <v>0.95</v>
       </c>
-      <c r="L51" s="6">
+      <c r="L52" s="6">
         <f t="shared" si="0"/>
         <v>0.95</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
         <v>49</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B53" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C53" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G52" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H52" s="1" t="s">
+      <c r="G53" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H53" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I52" s="15" t="s">
+      <c r="I53" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="J52" s="1">
-        <v>1</v>
-      </c>
-      <c r="K52">
+      <c r="J53" s="1">
+        <v>1</v>
+      </c>
+      <c r="K53">
         <v>4.25</v>
       </c>
-      <c r="L52" s="6">
+      <c r="L53" s="6">
         <f t="shared" si="0"/>
         <v>4.25</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="5">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="5">
         <v>50</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B54" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C54" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G53" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H53" s="1" t="s">
+      <c r="G54" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="I53" s="15" t="s">
+      <c r="I54" s="15" t="s">
         <v>319</v>
       </c>
-      <c r="J53" s="1">
-        <v>1</v>
-      </c>
-      <c r="K53">
+      <c r="J54" s="1">
+        <v>1</v>
+      </c>
+      <c r="K54">
         <v>6.66</v>
       </c>
-      <c r="L53" s="6">
+      <c r="L54" s="6">
         <f t="shared" si="0"/>
         <v>6.66</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
         <v>51</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B55" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C54" s="13" t="s">
+      <c r="C55" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G54" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H54" s="1" t="s">
+      <c r="G55" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H55" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I54" s="15" t="s">
+      <c r="I55" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="J54" s="1">
-        <v>1</v>
-      </c>
-      <c r="K54">
+      <c r="J55" s="1">
+        <v>1</v>
+      </c>
+      <c r="K55">
         <v>0.34</v>
       </c>
-      <c r="L54" s="6">
+      <c r="L55" s="6">
         <f t="shared" si="0"/>
         <v>0.34</v>
       </c>
     </row>
-    <row r="55" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="4">
+    <row r="56" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
         <v>52</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B56" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C55" s="13" t="s">
+      <c r="C56" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="E56" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="F56" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G55" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H55" s="1" t="s">
+      <c r="G56" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H56" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="I55" s="15" t="s">
+      <c r="I56" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="J55" s="1">
-        <v>1</v>
-      </c>
-      <c r="K55">
+      <c r="J56" s="1">
+        <v>1</v>
+      </c>
+      <c r="K56">
         <v>0.81</v>
       </c>
-      <c r="L55" s="6">
+      <c r="L56" s="6">
         <f t="shared" si="0"/>
         <v>0.81</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" s="4">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
         <v>53</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B57" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="C56" s="13" t="s">
+      <c r="C57" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="I56" s="15" t="s">
-        <v>342</v>
-      </c>
-      <c r="J56" s="1">
-        <v>1</v>
-      </c>
-      <c r="K56">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="L56" s="6">
-        <f t="shared" si="0"/>
-        <v>4.3099999999999996</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="5">
-        <v>54</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C57" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>171</v>
       </c>
       <c r="F57" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="I57" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="J57" s="1">
+        <v>1</v>
+      </c>
+      <c r="K57">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="L57" s="6">
+        <f t="shared" si="0"/>
+        <v>4.3099999999999996</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="5">
+        <v>54</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G57" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H57" s="1" t="s">
+      <c r="G58" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H58" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I57" s="15" t="s">
+      <c r="I58" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="J57" s="1">
-        <v>1</v>
-      </c>
-      <c r="K57">
+      <c r="J58" s="1">
+        <v>1</v>
+      </c>
+      <c r="K58">
         <v>1.58</v>
       </c>
-      <c r="L57" s="6">
+      <c r="L58" s="6">
         <f t="shared" si="0"/>
         <v>1.58</v>
       </c>
     </row>
-    <row r="58" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="4">
+    <row r="59" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
         <v>55</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B59" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C58" s="13" t="s">
+      <c r="C59" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="F59" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="G58" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H58" s="1" t="s">
+      <c r="G59" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H59" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="I58" s="15" t="s">
+      <c r="I59" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="J58" s="1">
-        <v>1</v>
-      </c>
-      <c r="K58">
+      <c r="J59" s="1">
+        <v>1</v>
+      </c>
+      <c r="K59">
         <v>2.59</v>
       </c>
-      <c r="L58" s="6">
+      <c r="L59" s="6">
         <f t="shared" si="0"/>
         <v>2.59</v>
       </c>
     </row>
-    <row r="59" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="5">
+    <row r="60" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="5">
         <v>56</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B60" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C59" s="13" t="s">
+      <c r="C60" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F59" s="1" t="s">
+      <c r="F60" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="G59" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H59" s="1" t="s">
+      <c r="G60" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H60" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="I59" s="15" t="s">
+      <c r="I60" s="15" t="s">
         <v>324</v>
       </c>
-      <c r="J59" s="1">
-        <v>1</v>
-      </c>
-      <c r="K59">
+      <c r="J60" s="1">
+        <v>1</v>
+      </c>
+      <c r="K60">
         <v>2.06</v>
       </c>
-      <c r="L59" s="6">
+      <c r="L60" s="6">
         <f t="shared" si="0"/>
         <v>2.06</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="4">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
         <v>57</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B61" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="C60" s="13" t="s">
+      <c r="C61" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="E61" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="F60" s="1">
+      <c r="F61" s="1">
         <v>7200</v>
       </c>
-      <c r="G60" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H60" s="1" t="s">
+      <c r="G61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H61" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="I60" s="15" t="s">
+      <c r="I61" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="J60" s="1">
+      <c r="J61" s="1">
         <v>4</v>
       </c>
-      <c r="K60">
+      <c r="K61">
         <v>0.68</v>
       </c>
-      <c r="L60" s="6">
+      <c r="L61" s="6">
         <f t="shared" si="0"/>
         <v>2.72</v>
       </c>

</xml_diff>

<commit_message>
Updated BOM file (removed R49, C117 and fixed C116 and J2).
</commit_message>
<xml_diff>
--- a/hardware/MainBoard/MainBoard_BOM.xlsx
+++ b/hardware/MainBoard/MainBoard_BOM.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="355">
   <si>
     <t>Item #</t>
   </si>
@@ -763,15 +763,6 @@
     <t>CAP CER 22PF 50V 5% NP0 0402</t>
   </si>
   <si>
-    <t>C1005X7R1C102K</t>
-  </si>
-  <si>
-    <t>445-6848-1-ND</t>
-  </si>
-  <si>
-    <t>CAP CER 1000PF 16V 10% X7R 0402</t>
-  </si>
-  <si>
     <t>C1005X5R1A475M</t>
   </si>
   <si>
@@ -793,9 +784,6 @@
     <t>CJS-1200TA</t>
   </si>
   <si>
-    <t>RJ45 connector</t>
-  </si>
-  <si>
     <t>MEZZANINE 1MM BTB RECPT 84CKT</t>
   </si>
   <si>
@@ -1105,7 +1093,34 @@
     <t>R14</t>
   </si>
   <si>
-    <t>R4, R11, R12, R13, R15, R16, R17, R18, R49, R74, R75</t>
+    <t>C116</t>
+  </si>
+  <si>
+    <t>445-2277-1-ND</t>
+  </si>
+  <si>
+    <t>C2012X7R2E102K</t>
+  </si>
+  <si>
+    <t>CAP CER 1000PF 250V 10% X7R 0805</t>
+  </si>
+  <si>
+    <t>C0805</t>
+  </si>
+  <si>
+    <t>553-1485-ND</t>
+  </si>
+  <si>
+    <t>J0011D21BNL</t>
+  </si>
+  <si>
+    <t>CONN PULSEJACK 1PORT 10/100B-TX</t>
+  </si>
+  <si>
+    <t>CON-RJ45-J0011D21BNL</t>
+  </si>
+  <si>
+    <t>R4, R11, R12, R13, R15, R16, R17, R18, R74, R75</t>
   </si>
 </sst>
 </file>
@@ -1599,8 +1614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1622,7 +1637,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -1757,7 +1772,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>57</v>
@@ -1766,19 +1781,19 @@
         <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="I6" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="J6" s="1">
         <v>18</v>
@@ -1835,7 +1850,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>41</v>
@@ -1964,16 +1979,16 @@
         <v>217</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="I11" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="J11" s="1">
         <v>7</v>
@@ -2058,38 +2073,38 @@
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>118</v>
+        <v>345</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>117</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>23</v>
+        <v>349</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>217</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>235</v>
+        <v>347</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>236</v>
+        <v>346</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>237</v>
+        <v>348</v>
       </c>
       <c r="J14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K14">
-        <v>0.08</v>
+        <v>0.17</v>
       </c>
       <c r="L14" s="6">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2097,7 +2112,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>63</v>
@@ -2109,16 +2124,16 @@
         <v>217</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="J15" s="1">
         <v>11</v>
@@ -2178,35 +2193,35 @@
         <v>146</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>145</v>
+        <v>353</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>145</v>
+        <v>353</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>149</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>150</v>
+        <v>351</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>148</v>
+        <v>350</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>245</v>
+        <v>352</v>
       </c>
       <c r="J17" s="1">
         <v>1</v>
       </c>
       <c r="K17">
-        <v>8.2100000000000009</v>
+        <v>7.1</v>
       </c>
       <c r="L17" s="6">
         <f t="shared" si="0"/>
-        <v>8.2100000000000009</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2235,7 +2250,7 @@
         <v>142</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="J18" s="1">
         <v>1</v>
@@ -2274,7 +2289,7 @@
         <v>132</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="J19" s="1">
         <v>1</v>
@@ -2313,7 +2328,7 @@
         <v>137</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="J20" s="1">
         <v>1</v>
@@ -2340,19 +2355,19 @@
         <v>85</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="J21" s="1">
         <v>2</v>
@@ -2385,10 +2400,10 @@
         <v>11</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="J22" s="1">
         <v>1</v>
@@ -2424,10 +2439,10 @@
         <v>11</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="J23" s="1">
         <v>1</v>
@@ -2454,7 +2469,7 @@
         <v>192</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>192</v>
@@ -2463,10 +2478,10 @@
         <v>11</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="J24" s="1">
         <v>1</v>
@@ -2493,19 +2508,19 @@
         <v>35</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="I25" s="15" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="J25" s="1">
         <v>6</v>
@@ -2532,19 +2547,19 @@
         <v>35</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="I26" s="15" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="J26" s="1">
         <v>8</v>
@@ -2571,19 +2586,19 @@
         <v>35</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="I27" s="15" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="J27" s="1">
         <v>6</v>
@@ -2610,19 +2625,19 @@
         <v>35</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="J28" s="1">
         <v>7</v>
@@ -2649,19 +2664,19 @@
         <v>35</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="I29" s="15" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="J29" s="1">
         <v>1</v>
@@ -2688,19 +2703,19 @@
         <v>35</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="J30" s="1">
         <v>2</v>
@@ -2727,19 +2742,19 @@
         <v>35</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="I31" s="15" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="J31" s="1">
         <v>4</v>
@@ -2766,19 +2781,19 @@
         <v>35</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="J32" s="1">
         <v>7</v>
@@ -2796,7 +2811,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="C33" s="13">
         <v>0</v>
@@ -2805,29 +2820,29 @@
         <v>35</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="I33" s="15" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="J33" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K33">
         <v>0.18099999999999999</v>
       </c>
       <c r="L33" s="6">
         <f t="shared" ref="L33" si="1">J33*K33</f>
-        <v>2.1719999999999997</v>
+        <v>1.9909999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2835,7 +2850,7 @@
         <v>30</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C34" s="14" t="s">
         <v>19</v>
@@ -2844,19 +2859,19 @@
         <v>35</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="G34" s="12" t="s">
         <v>11</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="I34" s="16" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="J34" s="12">
         <v>1</v>
@@ -2883,19 +2898,19 @@
         <v>35</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="I35" s="15" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="J35" s="1">
         <v>7</v>
@@ -2922,19 +2937,19 @@
         <v>35</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="I36" s="15" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="J36" s="1">
         <v>4</v>
@@ -2961,19 +2976,19 @@
         <v>35</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="J37" s="1">
         <v>1</v>
@@ -3000,19 +3015,19 @@
         <v>35</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="J38" s="1">
         <v>1</v>
@@ -3039,19 +3054,19 @@
         <v>35</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="I39" s="15" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="J39" s="1">
         <v>1</v>
@@ -3078,19 +3093,19 @@
         <v>35</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="I40" s="15" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="J40" s="1">
         <v>1</v>
@@ -3117,19 +3132,19 @@
         <v>35</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="I41" s="15" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="J41" s="1">
         <v>1</v>
@@ -3156,19 +3171,19 @@
         <v>35</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="I42" s="15" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="J42" s="1">
         <v>3</v>
@@ -3195,19 +3210,19 @@
         <v>35</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="I43" s="15" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="J43" s="1">
         <v>1</v>
@@ -3234,19 +3249,19 @@
         <v>35</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="I44" s="15" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="J44" s="1">
         <v>2</v>
@@ -3301,19 +3316,19 @@
         <v>200</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="I46" s="15" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="J46" s="1">
         <v>2</v>
@@ -3331,25 +3346,25 @@
         <v>43</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C47" s="13" t="s">
         <v>197</v>
       </c>
       <c r="D47" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>244</v>
-      </c>
       <c r="G47" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="I47" s="15" t="s">
         <v>199</v>
@@ -3391,7 +3406,7 @@
         <v>210</v>
       </c>
       <c r="I48" s="15" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="J48" s="1">
         <v>2</v>
@@ -3430,7 +3445,7 @@
         <v>206</v>
       </c>
       <c r="I49" s="15" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="J49" s="1">
         <v>2</v>
@@ -3469,7 +3484,7 @@
         <v>121</v>
       </c>
       <c r="I50" s="15" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="J50" s="1">
         <v>1</v>
@@ -3508,7 +3523,7 @@
         <v>190</v>
       </c>
       <c r="I51" s="15" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="J51" s="1">
         <v>2</v>
@@ -3625,7 +3640,7 @@
         <v>159</v>
       </c>
       <c r="I54" s="15" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="J54" s="1">
         <v>1</v>
@@ -3664,7 +3679,7 @@
         <v>103</v>
       </c>
       <c r="I55" s="15" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="J55" s="1">
         <v>1</v>
@@ -3703,7 +3718,7 @@
         <v>165</v>
       </c>
       <c r="I56" s="15" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="J56" s="1">
         <v>1</v>
@@ -3739,10 +3754,10 @@
         <v>11</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="I57" s="15" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="J57" s="1">
         <v>1</v>
@@ -3781,7 +3796,7 @@
         <v>170</v>
       </c>
       <c r="I58" s="15" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="J58" s="1">
         <v>1</v>
@@ -3820,7 +3835,7 @@
         <v>126</v>
       </c>
       <c r="I59" s="15" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="J59" s="1">
         <v>1</v>
@@ -3859,7 +3874,7 @@
         <v>176</v>
       </c>
       <c r="I60" s="15" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="J60" s="1">
         <v>1</v>
@@ -3895,10 +3910,10 @@
         <v>11</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="I61" s="15" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="J61" s="1">
         <v>4</v>

</xml_diff>